<commit_message>
Implement Narrative Event Selection
</commit_message>
<xml_diff>
--- a/Source/Narrative/Game Data.xlsx
+++ b/Source/Narrative/Game Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grayn\OneDrive\Documents\short\Under Choices\UnderChoices\Source\Narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B9A886-EECD-476B-ADCB-B1512E7562D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD441A6F-D526-4C1B-88A1-C95C629FBE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Media Posts" sheetId="1" r:id="rId1"/>
     <sheet name="Boss' Orders" sheetId="2" r:id="rId2"/>
+    <sheet name="Narrative Events" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="465">
   <si>
     <t>Post Number (Integer)</t>
   </si>
@@ -1397,6 +1398,30 @@
   </si>
   <si>
     <t>Number to Boost (Integer; 0 for "Don't Boost")</t>
+  </si>
+  <si>
+    <t>Event Number (Integer)</t>
+  </si>
+  <si>
+    <t>Effect (For Programmer's Reference)</t>
+  </si>
+  <si>
+    <t>None; test event</t>
+  </si>
+  <si>
+    <t>Name (String)</t>
+  </si>
+  <si>
+    <t>First Day</t>
+  </si>
+  <si>
+    <t>Collecting the Band</t>
+  </si>
+  <si>
+    <t>Scheduled Check-Up</t>
+  </si>
+  <si>
+    <t>Anti-Government Protest</t>
   </si>
 </sst>
 </file>
@@ -8777,8 +8802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C29F16F-EAFE-4B18-A8CA-D239C88544B3}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8913,4 +8938,111 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD59F98-9E92-490C-932F-B482BEFC87E4}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>461</v>
+      </c>
+      <c r="E2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E3" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>463</v>
+      </c>
+      <c r="E4" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>464</v>
+      </c>
+      <c r="E5" t="s">
+        <v>459</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement Updated Post Template
</commit_message>
<xml_diff>
--- a/Source/Narrative/Game Data.xlsx
+++ b/Source/Narrative/Game Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grayn\OneDrive\Documents\short\Under Choices\UnderChoices\Source\Narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD441A6F-D526-4C1B-88A1-C95C629FBE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6E6F5A-200F-4101-923E-2D28D3E0C45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1588,6 +1588,20 @@
     <tableColumn id="5" xr3:uid="{B3D3B5BA-85E2-49E3-A7E1-4F1317297D19}" name="Reaction (Any, Happy, Sad, Angry)"/>
     <tableColumn id="6" xr3:uid="{D0D4A58C-32DB-4F3D-B9FD-8C3465F8091F}" name="Narrative Subject (Government, Violence, Health, Radicalism)"/>
     <tableColumn id="7" xr3:uid="{44E759D3-CD71-49DA-8A1C-2BA34FC25D8E}" name="Publisher"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{103D08C7-DA4C-4F8C-80F6-5AFBF17EA556}" name="Table3" displayName="Table3" ref="A1:E5" totalsRowShown="0">
+  <autoFilter ref="A1:E5" xr:uid="{103D08C7-DA4C-4F8C-80F6-5AFBF17EA556}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{956ED486-AE82-4146-8CAD-99FBC1A02515}" name="Event Number (Integer)"/>
+    <tableColumn id="2" xr3:uid="{4EB92006-B123-4256-A786-0CF66AAAAD0E}" name="Day (Integer)"/>
+    <tableColumn id="3" xr3:uid="{70BC3B0A-D17B-46D4-8874-9C419DE11175}" name="Subject (Government, Violence, Health, Radicalism)"/>
+    <tableColumn id="4" xr3:uid="{98C7CB3D-0E3A-4329-8B8B-6DCE1B3ED87E}" name="Name (String)"/>
+    <tableColumn id="5" xr3:uid="{7D95D3ED-985E-4F7F-9C74-42E195DD8145}" name="Effect (For Programmer's Reference)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1858,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -1873,7 +1887,7 @@
     <col min="9" max="9" width="27.5703125" customWidth="1" outlineLevel="2"/>
     <col min="10" max="10" width="30.85546875" customWidth="1" outlineLevel="2"/>
     <col min="11" max="11" width="19" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="12" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="72.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -8945,16 +8959,16 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -9044,5 +9058,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix Boss Orders Bug
</commit_message>
<xml_diff>
--- a/Source/Narrative/Game Data.xlsx
+++ b/Source/Narrative/Game Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtsp1\Documents\GitHub\The-Cool-Guys\UnderChoices\Source\Narrative\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grayn\OneDrive\Documents\short\Under Choices\UnderChoices\Source\Narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E04A19-207D-4E55-A282-1E14B3804981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523FD847-4FC0-4622-A5EA-0C65E563476D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Media Posts" sheetId="1" r:id="rId1"/>
@@ -9988,8 +9988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C29F16F-EAFE-4B18-A8CA-D239C88544B3}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Engagement w/ New hashtags
</commit_message>
<xml_diff>
--- a/Source/Narrative/Game Data.xlsx
+++ b/Source/Narrative/Game Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mptun\Desktop\UnderChoices\Source\Narrative\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtsp1\Documents\GitHub\The-Cool-Guys\UnderChoices\Source\Narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73689B42-8DF5-473F-86E8-853E6C36264C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBE6B87-B967-400E-8219-715BC03CD529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Media Posts" sheetId="1" r:id="rId1"/>
@@ -2311,8 +2311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -2394,17 +2394,17 @@
       </c>
       <c r="G2" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G2" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v xml:space="preserve">Saviours </v>
       </c>
       <c r="H2" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H2" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>InGoodHands</v>
       </c>
       <c r="I2">
         <v>75</v>
       </c>
       <c r="J2">
-        <v>16000</v>
+        <v>11000</v>
       </c>
       <c r="K2" s="1">
         <v>100</v>
@@ -2434,21 +2434,21 @@
       </c>
       <c r="F3" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F3" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>KeepThemIN!</v>
+        <v>RepeatElection</v>
       </c>
       <c r="G3" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G3" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>KeepThemIN!</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="H3" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H3" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>People'sVoice</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="I3">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="J3">
-        <v>28000</v>
+        <v>15000</v>
       </c>
       <c r="K3" s="1">
         <v>156</v>
@@ -2478,7 +2478,7 @@
       </c>
       <c r="F4" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F4" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>WhatAJoke</v>
       </c>
       <c r="G4" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G4" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -2489,7 +2489,7 @@
         <v>I'maSitDown</v>
       </c>
       <c r="I4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J4">
         <v>15000</v>
@@ -2522,18 +2522,18 @@
       </c>
       <c r="F5" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F5" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="G5" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G5" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>WhatAJoke</v>
       </c>
       <c r="H5" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H5" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
         <v>NoFaith</v>
       </c>
       <c r="I5">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="J5">
         <v>16000</v>
@@ -2566,21 +2566,21 @@
       </c>
       <c r="F6" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F6" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="G6" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>BurnItDOWN</v>
       </c>
       <c r="H6" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H6" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>BurnItDOWN</v>
       </c>
       <c r="I6">
-        <v>117</v>
+        <v>200</v>
       </c>
       <c r="J6">
-        <v>28000</v>
+        <v>30000</v>
       </c>
       <c r="K6" s="1">
         <v>121</v>
@@ -2610,21 +2610,21 @@
       </c>
       <c r="F7" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F7" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="G7" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G7" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RiotTIME</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="H7" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="I7">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="J7">
-        <v>15000</v>
+        <v>28000</v>
       </c>
       <c r="K7" s="1">
         <v>131</v>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="F8" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F8" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>Justified!</v>
       </c>
       <c r="G8" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G8" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -2662,13 +2662,13 @@
       </c>
       <c r="H8" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H8" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>StrongerTogether</v>
       </c>
       <c r="I8">
         <v>75</v>
       </c>
       <c r="J8">
-        <v>16000</v>
+        <v>10000</v>
       </c>
       <c r="K8" s="1">
         <v>98</v>
@@ -2698,21 +2698,21 @@
       </c>
       <c r="F9" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F9" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="G9" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G9" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>StrongerTogether</v>
       </c>
       <c r="H9" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H9" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>Hero</v>
       </c>
       <c r="I9">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="J9">
-        <v>28000</v>
+        <v>13000</v>
       </c>
       <c r="K9" s="1">
         <v>132</v>
@@ -2742,21 +2742,21 @@
       </c>
       <c r="F10" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>PrayForThem</v>
       </c>
       <c r="G10" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G10" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>FreeThem</v>
       </c>
       <c r="H10" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H10" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>Lowlife</v>
       </c>
       <c r="I10">
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="J10">
-        <v>15000</v>
+        <v>16000</v>
       </c>
       <c r="K10" s="1">
         <v>149</v>
@@ -2786,21 +2786,21 @@
       </c>
       <c r="F11" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="G11" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G11" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>TooSoon</v>
       </c>
       <c r="H11" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H11" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>SoTragic</v>
       </c>
       <c r="I11">
-        <v>75</v>
+        <v>175</v>
       </c>
       <c r="J11">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="K11" s="1">
         <v>89</v>
@@ -2830,21 +2830,21 @@
       </c>
       <c r="F12" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>DeathCollection</v>
       </c>
       <c r="G12" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G12" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>AskingForIt</v>
       </c>
       <c r="H12" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H12" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="I12">
-        <v>117</v>
+        <v>325</v>
       </c>
       <c r="J12">
-        <v>28000</v>
+        <v>32000</v>
       </c>
       <c r="K12" s="1">
         <v>69</v>
@@ -2874,21 +2874,21 @@
       </c>
       <c r="F13" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="G13" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G13" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>AskingForIt</v>
       </c>
       <c r="H13" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H13" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="I13">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="J13">
-        <v>15000</v>
+        <v>28000</v>
       </c>
       <c r="K13" s="1">
         <v>50</v>
@@ -2918,21 +2918,21 @@
       </c>
       <c r="F14" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>100Sober</v>
       </c>
       <c r="G14" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G14" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="H14" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H14" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>Recovered:)</v>
       </c>
       <c r="I14">
         <v>75</v>
       </c>
       <c r="J14">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="K14" s="1">
         <v>134</v>
@@ -2966,17 +2966,17 @@
       </c>
       <c r="G15" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G15" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="H15" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H15" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>BestWishes</v>
       </c>
       <c r="I15">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="J15">
-        <v>28000</v>
+        <v>14000</v>
       </c>
       <c r="K15" s="1">
         <v>78</v>
@@ -3006,18 +3006,18 @@
       </c>
       <c r="F16" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F16" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>Drained</v>
       </c>
       <c r="G16" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="H16" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H16" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
         <v>WeLostThem</v>
       </c>
       <c r="I16">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="J16">
         <v>15000</v>
@@ -3050,7 +3050,7 @@
       </c>
       <c r="F17" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F17" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>God'sPlan</v>
       </c>
       <c r="G17" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G17" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -3058,10 +3058,10 @@
       </c>
       <c r="H17" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H17" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="I17">
-        <v>75</v>
+        <v>175</v>
       </c>
       <c r="J17">
         <v>16000</v>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="F18" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F18" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="G18" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -3102,13 +3102,13 @@
       </c>
       <c r="H18" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H18" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="I18">
-        <v>117</v>
+        <v>350</v>
       </c>
       <c r="J18">
-        <v>28000</v>
+        <v>26000</v>
       </c>
       <c r="K18" s="1">
         <v>175</v>
@@ -3138,21 +3138,21 @@
       </c>
       <c r="F19" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F19" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>Refund</v>
       </c>
       <c r="G19" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>CrapStaff</v>
       </c>
       <c r="H19" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H19" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="I19">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="J19">
-        <v>15000</v>
+        <v>28000</v>
       </c>
       <c r="K19" s="1">
         <v>91</v>
@@ -3182,21 +3182,21 @@
       </c>
       <c r="F20" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F20" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="G20" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>CommunityBuild</v>
+        <v>WEStrong</v>
       </c>
       <c r="H20" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H20" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="I20">
         <v>75</v>
       </c>
       <c r="J20">
-        <v>16000</v>
+        <v>11000</v>
       </c>
       <c r="K20" s="1">
         <v>150</v>
@@ -3226,21 +3226,21 @@
       </c>
       <c r="F21" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F21" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="G21" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="H21" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H21" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="I21">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="J21">
-        <v>28000</v>
+        <v>13000</v>
       </c>
       <c r="K21" s="1">
         <v>110</v>
@@ -3270,18 +3270,18 @@
       </c>
       <c r="F22" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F22" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>Outcast</v>
       </c>
       <c r="G22" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>SplitUp</v>
       </c>
       <c r="H22" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H22" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>SplitUp</v>
       </c>
       <c r="I22">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="J22">
         <v>15000</v>
@@ -3314,18 +3314,18 @@
       </c>
       <c r="F23" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F23" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>SplitUp</v>
       </c>
       <c r="G23" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WeNeedChange</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="H23" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H23" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="I23">
-        <v>75</v>
+        <v>200</v>
       </c>
       <c r="J23">
         <v>16000</v>
@@ -3358,21 +3358,21 @@
       </c>
       <c r="F24" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F24" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>OurLastHope</v>
       </c>
       <c r="G24" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G24" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="H24" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H24" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="I24">
-        <v>117</v>
+        <v>400</v>
       </c>
       <c r="J24">
-        <v>28000</v>
+        <v>31000</v>
       </c>
       <c r="K24" s="1">
         <v>147</v>
@@ -3402,21 +3402,21 @@
       </c>
       <c r="F25" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F25" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>Messiah</v>
       </c>
       <c r="G25" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G25" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>OurLastHope</v>
       </c>
       <c r="H25" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H25" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
         <v>OurLastHope</v>
       </c>
       <c r="I25">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="J25">
-        <v>15000</v>
+        <v>28000</v>
       </c>
       <c r="K25" s="1">
         <v>90</v>
@@ -3450,17 +3450,17 @@
       </c>
       <c r="G26" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G26" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>People'sVoice</v>
       </c>
       <c r="H26" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H26" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
         <v>InGoodHands</v>
       </c>
       <c r="I26">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J26">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K26" s="1">
         <v>100</v>
@@ -3490,21 +3490,21 @@
       </c>
       <c r="F27" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F27" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="G27" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G27" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>KeepThemIN!</v>
+        <v>ReElect!!!</v>
       </c>
       <c r="H27" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H27" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
         <v xml:space="preserve">Saviours </v>
       </c>
       <c r="I27">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J27">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K27" s="1">
         <v>156</v>
@@ -3534,21 +3534,21 @@
       </c>
       <c r="F28" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F28" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="G28" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G28" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="H28" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H28" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>NoFaith</v>
       </c>
       <c r="I28">
         <v>100</v>
       </c>
       <c r="J28">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K28" s="1">
         <v>80</v>
@@ -3578,21 +3578,21 @@
       </c>
       <c r="F29" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F29" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="G29" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G29" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>ItsOver</v>
       </c>
       <c r="H29" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H29" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="I29">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J29">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K29" s="1">
         <v>75</v>
@@ -3622,21 +3622,21 @@
       </c>
       <c r="F30" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F30" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="G30" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G30" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>CoupDeTahhh</v>
+        <v>ToTheTorches!</v>
       </c>
       <c r="H30" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H30" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
         <v>ToTheTorches!</v>
       </c>
       <c r="I30">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J30">
-        <v>10000</v>
+        <v>30000</v>
       </c>
       <c r="K30" s="1">
         <v>121</v>
@@ -3666,21 +3666,21 @@
       </c>
       <c r="F31" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F31" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>RaidingNight</v>
       </c>
       <c r="G31" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G31" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="H31" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H31" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="I31">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J31">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K31" s="1">
         <v>131</v>
@@ -3714,14 +3714,14 @@
       </c>
       <c r="G32" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G32" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>BeSafe</v>
       </c>
       <c r="H32" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H32" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>BeSafe</v>
       </c>
       <c r="I32">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J32">
         <v>10000</v>
@@ -3754,11 +3754,11 @@
       </c>
       <c r="F33" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F33" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>Justice</v>
       </c>
       <c r="G33" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G33" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>Justice</v>
       </c>
       <c r="H33" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H33" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -3768,7 +3768,7 @@
         <v>100</v>
       </c>
       <c r="J33">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K33" s="1">
         <v>132</v>
@@ -3798,21 +3798,21 @@
       </c>
       <c r="F34" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F34" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>SoTragic</v>
       </c>
       <c r="G34" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G34" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>PrayForThem</v>
       </c>
       <c r="H34" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H34" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>Lowlife</v>
       </c>
       <c r="I34">
-        <v>100</v>
+        <v>225</v>
       </c>
       <c r="J34">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K34" s="1">
         <v>149</v>
@@ -3842,21 +3842,21 @@
       </c>
       <c r="F35" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F35" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>FreeThem</v>
       </c>
       <c r="G35" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G35" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>WhatAShame</v>
       </c>
       <c r="H35" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H35" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>TooSoon</v>
       </c>
       <c r="I35">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J35">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K35" s="1">
         <v>89</v>
@@ -3886,21 +3886,21 @@
       </c>
       <c r="F36" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F36" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="G36" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G36" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>AskingForIt</v>
       </c>
       <c r="H36" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H36" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
         <v>DeathCollection</v>
       </c>
       <c r="I36">
-        <v>100</v>
+        <v>325</v>
       </c>
       <c r="J36">
-        <v>10000</v>
+        <v>32000</v>
       </c>
       <c r="K36" s="1">
         <v>69</v>
@@ -3930,21 +3930,21 @@
       </c>
       <c r="F37" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F37" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>Despicable!</v>
       </c>
       <c r="G37" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G37" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>Despicable!</v>
       </c>
       <c r="H37" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H37" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>DeathCollection</v>
       </c>
       <c r="I37">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J37">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K37" s="1">
         <v>50</v>
@@ -3974,21 +3974,21 @@
       </c>
       <c r="F38" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F38" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>100Sober</v>
       </c>
       <c r="G38" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G38" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Hugs&amp;Kisses</v>
+        <v>BestWishes</v>
       </c>
       <c r="H38" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H38" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>BackToUs</v>
       </c>
       <c r="I38">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J38">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K38" s="1">
         <v>134</v>
@@ -4018,21 +4018,21 @@
       </c>
       <c r="F39" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F39" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>100Sober</v>
+        <v>BestWishes</v>
       </c>
       <c r="G39" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G39" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="H39" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H39" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="I39">
         <v>100</v>
       </c>
       <c r="J39">
-        <v>10000</v>
+        <v>14000</v>
       </c>
       <c r="K39" s="1">
         <v>78</v>
@@ -4066,17 +4066,17 @@
       </c>
       <c r="G40" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G40" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="H40" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H40" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>Depressing</v>
       </c>
       <c r="I40">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J40">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K40" s="1">
         <v>145</v>
@@ -4106,21 +4106,21 @@
       </c>
       <c r="F41" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F41" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>I'mSoLost</v>
       </c>
       <c r="G41" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G41" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Depressing</v>
+        <v>God'sPlan</v>
       </c>
       <c r="H41" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H41" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="I41">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J41">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K41" s="1">
         <v>82</v>
@@ -4154,17 +4154,17 @@
       </c>
       <c r="G42" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G42" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>Refund</v>
       </c>
       <c r="H42" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H42" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
         <v>CrapStaff</v>
       </c>
       <c r="I42">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="J42">
-        <v>10000</v>
+        <v>26000</v>
       </c>
       <c r="K42" s="1">
         <v>175</v>
@@ -4194,21 +4194,21 @@
       </c>
       <c r="F43" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F43" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>CrapStaff</v>
       </c>
       <c r="G43" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G43" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="H43" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H43" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="I43">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="J43">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K43" s="1">
         <v>91</v>
@@ -4238,21 +4238,21 @@
       </c>
       <c r="F44" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F44" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>WEStrong</v>
       </c>
       <c r="G44" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G44" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>ALWAYSSupport</v>
       </c>
       <c r="H44" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H44" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WEStrong</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="I44">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J44">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K44" s="1">
         <v>150</v>
@@ -4286,17 +4286,17 @@
       </c>
       <c r="G45" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G45" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="H45" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H45" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
         <v>JoinTheCAUSE</v>
       </c>
       <c r="I45">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J45">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K45" s="1">
         <v>110</v>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="F46" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F46" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>SplitUp</v>
       </c>
       <c r="G46" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G46" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -4334,13 +4334,13 @@
       </c>
       <c r="H46" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H46" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>Outcast</v>
       </c>
       <c r="I46">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J46">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K46" s="1">
         <v>60</v>
@@ -4374,17 +4374,17 @@
       </c>
       <c r="G47" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G47" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WeNeedChange</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="H47" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H47" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
         <v>SplitUp</v>
       </c>
       <c r="I47">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J47">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K47" s="1">
         <v>70</v>
@@ -4414,21 +4414,21 @@
       </c>
       <c r="F48" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F48" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="G48" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G48" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>OurLastHope</v>
       </c>
       <c r="H48" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H48" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>Messiah</v>
       </c>
       <c r="I48">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="J48">
-        <v>10000</v>
+        <v>31000</v>
       </c>
       <c r="K48" s="1">
         <v>147</v>
@@ -4458,21 +4458,21 @@
       </c>
       <c r="F49" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F49" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>NecessaryEvil</v>
+        <v>OurLastHope</v>
       </c>
       <c r="G49" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G49" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="H49" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H49" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>Messiah</v>
       </c>
       <c r="I49">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J49">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K49" s="1">
         <v>90</v>
@@ -4502,21 +4502,21 @@
       </c>
       <c r="F50" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F50" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="G50" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G50" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>People'sVoice</v>
       </c>
       <c r="H50" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H50" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
         <v>VoteAgain</v>
       </c>
       <c r="I50">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J50">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K50" s="1">
         <v>100</v>
@@ -4546,21 +4546,21 @@
       </c>
       <c r="F51" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F51" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="G51" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G51" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>People'sVoice</v>
       </c>
       <c r="H51" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H51" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>InGoodHands</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="I51">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J51">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K51" s="1">
         <v>156</v>
@@ -4590,11 +4590,11 @@
       </c>
       <c r="F52" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F52" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="G52" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G52" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>ItsOver</v>
       </c>
       <c r="H52" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H52" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -4604,7 +4604,7 @@
         <v>100</v>
       </c>
       <c r="J52">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K52" s="1">
         <v>80</v>
@@ -4634,21 +4634,21 @@
       </c>
       <c r="F53" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F53" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>NoFaith</v>
       </c>
       <c r="G53" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G53" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>NoFaith</v>
       </c>
       <c r="H53" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H53" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>NoFaith</v>
       </c>
       <c r="I53">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J53">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K53" s="1">
         <v>75</v>
@@ -4682,17 +4682,17 @@
       </c>
       <c r="G54" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G54" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>RaidingNight</v>
       </c>
       <c r="H54" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H54" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="I54">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J54">
-        <v>10000</v>
+        <v>30000</v>
       </c>
       <c r="K54" s="1">
         <v>121</v>
@@ -4722,21 +4722,21 @@
       </c>
       <c r="F55" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F55" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RiotTIME</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="G55" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G55" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="H55" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H55" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="I55">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J55">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K55" s="1">
         <v>131</v>
@@ -4766,18 +4766,18 @@
       </c>
       <c r="F56" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F56" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FightBackTeam!</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="G56" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G56" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FightBackTeam!</v>
+        <v>StrongerTogether</v>
       </c>
       <c r="H56" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H56" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
         <v>Justice</v>
       </c>
       <c r="I56">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J56">
         <v>10000</v>
@@ -4810,21 +4810,21 @@
       </c>
       <c r="F57" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F57" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="G57" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G57" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>Justified!</v>
       </c>
       <c r="H57" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H57" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>StrongerTogether</v>
       </c>
       <c r="I57">
         <v>100</v>
       </c>
       <c r="J57">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K57" s="1">
         <v>132</v>
@@ -4854,21 +4854,21 @@
       </c>
       <c r="F58" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F58" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>SoTragic</v>
       </c>
       <c r="G58" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G58" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>Lowlife</v>
       </c>
       <c r="H58" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H58" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>FreeThem</v>
       </c>
       <c r="I58">
-        <v>100</v>
+        <v>225</v>
       </c>
       <c r="J58">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K58" s="1">
         <v>149</v>
@@ -4898,21 +4898,21 @@
       </c>
       <c r="F59" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F59" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>SoTragic</v>
       </c>
       <c r="G59" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G59" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>Pathetic</v>
       </c>
       <c r="H59" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H59" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>PrayForThem</v>
       </c>
       <c r="I59">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J59">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K59" s="1">
         <v>89</v>
@@ -4946,17 +4946,17 @@
       </c>
       <c r="G60" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G60" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="H60" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H60" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
         <v>DeathCollection</v>
       </c>
       <c r="I60">
-        <v>100</v>
+        <v>325</v>
       </c>
       <c r="J60">
-        <v>10000</v>
+        <v>32000</v>
       </c>
       <c r="K60" s="1">
         <v>69</v>
@@ -4986,21 +4986,21 @@
       </c>
       <c r="F61" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F61" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>Despicable!</v>
       </c>
       <c r="G61" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G61" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="H61" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H61" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="I61">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J61">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K61" s="1">
         <v>50</v>
@@ -5030,21 +5030,21 @@
       </c>
       <c r="F62" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F62" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="G62" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G62" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>MadeIt</v>
       </c>
       <c r="H62" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H62" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
         <v>Hugs&amp;Kisses</v>
       </c>
       <c r="I62">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J62">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K62" s="1">
         <v>134</v>
@@ -5074,21 +5074,21 @@
       </c>
       <c r="F63" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F63" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>100Sober</v>
       </c>
       <c r="G63" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G63" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>ThankGod</v>
       </c>
       <c r="H63" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H63" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>MadeIt</v>
       </c>
       <c r="I63">
         <v>100</v>
       </c>
       <c r="J63">
-        <v>10000</v>
+        <v>14000</v>
       </c>
       <c r="K63" s="1">
         <v>78</v>
@@ -5118,21 +5118,21 @@
       </c>
       <c r="F64" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F64" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>Depressing</v>
       </c>
       <c r="G64" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G64" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>HardTimes</v>
       </c>
       <c r="H64" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H64" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>HELPME</v>
       </c>
       <c r="I64">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J64">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K64" s="1">
         <v>145</v>
@@ -5162,21 +5162,21 @@
       </c>
       <c r="F65" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F65" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>Drained</v>
       </c>
       <c r="G65" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G65" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>HELPME</v>
       </c>
       <c r="H65" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H65" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>HELPME</v>
       </c>
       <c r="I65">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J65">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K65" s="1">
         <v>82</v>
@@ -5206,21 +5206,21 @@
       </c>
       <c r="F66" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F66" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="G66" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G66" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>CrapStaff</v>
       </c>
       <c r="H66" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H66" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="I66">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="J66">
-        <v>10000</v>
+        <v>26000</v>
       </c>
       <c r="K66" s="1">
         <v>175</v>
@@ -5254,17 +5254,17 @@
       </c>
       <c r="G67" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G67" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>CrapStaff</v>
       </c>
       <c r="H67" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H67" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="I67">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="J67">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K67" s="1">
         <v>91</v>
@@ -5294,21 +5294,21 @@
       </c>
       <c r="F68" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F68" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>CommunityBuild</v>
+        <v>WEStrong</v>
       </c>
       <c r="G68" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G68" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>WEStrong</v>
       </c>
       <c r="H68" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H68" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="I68">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J68">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K68" s="1">
         <v>150</v>
@@ -5338,21 +5338,21 @@
       </c>
       <c r="F69" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F69" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="G69" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G69" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>WEStrong</v>
       </c>
       <c r="H69" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H69" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>WEStrong</v>
       </c>
       <c r="I69">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J69">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K69" s="1">
         <v>110</v>
@@ -5382,21 +5382,21 @@
       </c>
       <c r="F70" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F70" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="G70" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G70" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>SplitUp</v>
       </c>
       <c r="H70" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H70" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>SplitUp</v>
       </c>
       <c r="I70">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J70">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K70" s="1">
         <v>60</v>
@@ -5426,7 +5426,7 @@
       </c>
       <c r="F71" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F71" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="G71" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G71" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -5434,13 +5434,13 @@
       </c>
       <c r="H71" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H71" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="I71">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J71">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K71" s="1">
         <v>70</v>
@@ -5470,7 +5470,7 @@
       </c>
       <c r="F72" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F72" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="G72" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G72" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -5478,13 +5478,13 @@
       </c>
       <c r="H72" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H72" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>OurLastHope</v>
       </c>
       <c r="I72">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="J72">
-        <v>10000</v>
+        <v>31000</v>
       </c>
       <c r="K72" s="1">
         <v>147</v>
@@ -5514,21 +5514,21 @@
       </c>
       <c r="F73" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F73" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>NecessaryEvil</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="G73" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G73" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="H73" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H73" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="I73">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J73">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K73" s="1">
         <v>90</v>
@@ -5558,21 +5558,21 @@
       </c>
       <c r="F74" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F74" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>People'sVoice</v>
       </c>
       <c r="G74" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G74" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>ReElect!!!</v>
       </c>
       <c r="H74" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H74" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>VoteAgain</v>
       </c>
       <c r="I74">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J74">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K74" s="1">
         <v>100</v>
@@ -5602,21 +5602,21 @@
       </c>
       <c r="F75" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F75" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="G75" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G75" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v>People'sVoice</v>
       </c>
       <c r="H75" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H75" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="I75">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J75">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K75" s="1">
         <v>156</v>
@@ -5646,21 +5646,21 @@
       </c>
       <c r="F76" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F76" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="G76" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G76" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="H76" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H76" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>I'maSitDown</v>
       </c>
       <c r="I76">
         <v>100</v>
       </c>
       <c r="J76">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K76" s="1">
         <v>80</v>
@@ -5690,7 +5690,7 @@
       </c>
       <c r="F77" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F77" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="G77" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G77" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -5698,13 +5698,13 @@
       </c>
       <c r="H77" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H77" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>NoFaith</v>
       </c>
       <c r="I77">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J77">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K77" s="1">
         <v>75</v>
@@ -5734,21 +5734,21 @@
       </c>
       <c r="F78" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F78" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>ToTheTorches!</v>
       </c>
       <c r="G78" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G78" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RiotTIME</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="H78" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H78" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="I78">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J78">
-        <v>10000</v>
+        <v>30000</v>
       </c>
       <c r="K78" s="1">
         <v>121</v>
@@ -5778,7 +5778,7 @@
       </c>
       <c r="F79" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F79" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>RiotTIME</v>
       </c>
       <c r="G79" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G79" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -5786,13 +5786,13 @@
       </c>
       <c r="H79" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H79" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>CoupDeTahhh</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="I79">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J79">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K79" s="1">
         <v>131</v>
@@ -5826,14 +5826,14 @@
       </c>
       <c r="G80" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G80" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>StrongerTogether</v>
       </c>
       <c r="H80" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H80" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>BeSafe</v>
       </c>
       <c r="I80">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J80">
         <v>10000</v>
@@ -5870,17 +5870,17 @@
       </c>
       <c r="G81" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G81" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="H81" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H81" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>Justified!</v>
       </c>
       <c r="I81">
         <v>100</v>
       </c>
       <c r="J81">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K81" s="1">
         <v>132</v>
@@ -5910,21 +5910,21 @@
       </c>
       <c r="F82" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F82" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>TooSoon</v>
       </c>
       <c r="G82" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G82" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>WhatAShame</v>
       </c>
       <c r="H82" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H82" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>Pathetic</v>
       </c>
       <c r="I82">
-        <v>100</v>
+        <v>225</v>
       </c>
       <c r="J82">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K82" s="1">
         <v>149</v>
@@ -5958,17 +5958,17 @@
       </c>
       <c r="G83" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G83" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>FreeThem</v>
       </c>
       <c r="H83" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H83" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>Pathetic</v>
       </c>
       <c r="I83">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J83">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K83" s="1">
         <v>89</v>
@@ -5998,21 +5998,21 @@
       </c>
       <c r="F84" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F84" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="G84" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G84" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="H84" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H84" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="I84">
-        <v>100</v>
+        <v>325</v>
       </c>
       <c r="J84">
-        <v>10000</v>
+        <v>32000</v>
       </c>
       <c r="K84" s="1">
         <v>69</v>
@@ -6042,21 +6042,21 @@
       </c>
       <c r="F85" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F85" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="G85" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G85" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>Despicable!</v>
       </c>
       <c r="H85" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H85" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="I85">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J85">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K85" s="1">
         <v>50</v>
@@ -6090,17 +6090,17 @@
       </c>
       <c r="G86" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G86" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>ThankGod</v>
       </c>
       <c r="H86" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H86" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>100Sober</v>
       </c>
       <c r="I86">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J86">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K86" s="1">
         <v>134</v>
@@ -6134,17 +6134,17 @@
       </c>
       <c r="G87" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G87" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>100Sober</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="H87" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H87" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="I87">
         <v>100</v>
       </c>
       <c r="J87">
-        <v>10000</v>
+        <v>14000</v>
       </c>
       <c r="K87" s="1">
         <v>78</v>
@@ -6178,17 +6178,17 @@
       </c>
       <c r="G88" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G88" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>God'sPlan</v>
       </c>
       <c r="H88" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H88" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>WeLostThem</v>
       </c>
       <c r="I88">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J88">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K88" s="1">
         <v>145</v>
@@ -6218,21 +6218,21 @@
       </c>
       <c r="F89" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F89" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>Depressing</v>
       </c>
       <c r="G89" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G89" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>HardTimes</v>
       </c>
       <c r="H89" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H89" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
         <v>Drained</v>
       </c>
       <c r="I89">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J89">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K89" s="1">
         <v>82</v>
@@ -6262,7 +6262,7 @@
       </c>
       <c r="F90" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F90" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>CrapStaff</v>
       </c>
       <c r="G90" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G90" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -6270,13 +6270,13 @@
       </c>
       <c r="H90" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H90" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="I90">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="J90">
-        <v>10000</v>
+        <v>26000</v>
       </c>
       <c r="K90" s="1">
         <v>175</v>
@@ -6306,7 +6306,7 @@
       </c>
       <c r="F91" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F91" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="G91" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G91" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -6314,13 +6314,13 @@
       </c>
       <c r="H91" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H91" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="I91">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="J91">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K91" s="1">
         <v>91</v>
@@ -6350,21 +6350,21 @@
       </c>
       <c r="F92" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F92" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="G92" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G92" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>ALWAYSSupport</v>
       </c>
       <c r="H92" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H92" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>CommunityBuild</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="I92">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J92">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K92" s="1">
         <v>150</v>
@@ -6394,21 +6394,21 @@
       </c>
       <c r="F93" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F93" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="G93" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G93" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="H93" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H93" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="I93">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J93">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K93" s="1">
         <v>110</v>
@@ -6438,21 +6438,21 @@
       </c>
       <c r="F94" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F94" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WeNeedChange</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="G94" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G94" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>Desperate</v>
       </c>
       <c r="H94" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H94" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>SplitUp</v>
       </c>
       <c r="I94">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J94">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K94" s="1">
         <v>60</v>
@@ -6482,21 +6482,21 @@
       </c>
       <c r="F95" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F95" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="G95" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G95" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>Outcast</v>
       </c>
       <c r="H95" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H95" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>Desperate</v>
       </c>
       <c r="I95">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J95">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K95" s="1">
         <v>70</v>
@@ -6526,21 +6526,21 @@
       </c>
       <c r="F96" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F96" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="G96" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G96" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>Messiah</v>
       </c>
       <c r="H96" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H96" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="I96">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="J96">
-        <v>10000</v>
+        <v>31000</v>
       </c>
       <c r="K96" s="1">
         <v>147</v>
@@ -6570,21 +6570,21 @@
       </c>
       <c r="F97" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F97" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="G97" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G97" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="H97" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H97" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>Messiah</v>
       </c>
       <c r="I97">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J97">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K97" s="1">
         <v>90</v>
@@ -6614,21 +6614,21 @@
       </c>
       <c r="F98" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F98" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v xml:space="preserve">Saviours </v>
       </c>
       <c r="G98" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G98" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v xml:space="preserve">Saviours </v>
       </c>
       <c r="H98" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H98" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>InGoodHands</v>
       </c>
       <c r="I98">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J98">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K98" s="1">
         <v>100</v>
@@ -6662,17 +6662,17 @@
       </c>
       <c r="G99" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G99" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>InGoodHands</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="H99" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H99" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v xml:space="preserve">Saviours </v>
       </c>
       <c r="I99">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J99">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K99" s="1">
         <v>156</v>
@@ -6702,7 +6702,7 @@
       </c>
       <c r="F100" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F100" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>WhatAJoke</v>
       </c>
       <c r="G100" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G100" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -6710,13 +6710,13 @@
       </c>
       <c r="H100" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H100" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="I100">
         <v>100</v>
       </c>
       <c r="J100">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K100" s="1">
         <v>80</v>
@@ -6746,21 +6746,21 @@
       </c>
       <c r="F101" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F101" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="G101" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G101" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>ItsOver</v>
       </c>
       <c r="H101" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H101" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>ItsOver</v>
       </c>
       <c r="I101">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J101">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K101" s="1">
         <v>75</v>
@@ -6794,17 +6794,17 @@
       </c>
       <c r="G102" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G102" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="H102" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H102" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
         <v>Pitchforks!!!</v>
       </c>
       <c r="I102">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J102">
-        <v>10000</v>
+        <v>30000</v>
       </c>
       <c r="K102" s="1">
         <v>121</v>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="F103" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F103" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="G103" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G103" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -6842,13 +6842,13 @@
       </c>
       <c r="H103" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H103" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="I103">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J103">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K103" s="1">
         <v>131</v>
@@ -6878,18 +6878,18 @@
       </c>
       <c r="F104" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F104" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="G104" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G104" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>BeSafe</v>
       </c>
       <c r="H104" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H104" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FightBackTeam!</v>
+        <v>Hero</v>
       </c>
       <c r="I104">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J104">
         <v>10000</v>
@@ -6922,7 +6922,7 @@
       </c>
       <c r="F105" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F105" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FightBackTeam!</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="G105" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G105" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -6930,13 +6930,13 @@
       </c>
       <c r="H105" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H105" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>Justified!</v>
       </c>
       <c r="I105">
         <v>100</v>
       </c>
       <c r="J105">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K105" s="1">
         <v>132</v>
@@ -6966,21 +6966,21 @@
       </c>
       <c r="F106" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F106" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="G106" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G106" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>FreeThem</v>
       </c>
       <c r="H106" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H106" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>FreeThem</v>
       </c>
       <c r="I106">
-        <v>100</v>
+        <v>225</v>
       </c>
       <c r="J106">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K106" s="1">
         <v>149</v>
@@ -7014,17 +7014,17 @@
       </c>
       <c r="G107" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G107" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>WhatAShame</v>
       </c>
       <c r="H107" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H107" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>SoTragic</v>
       </c>
       <c r="I107">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J107">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K107" s="1">
         <v>89</v>
@@ -7054,21 +7054,21 @@
       </c>
       <c r="F108" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F108" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="G108" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G108" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="H108" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H108" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>PaybackTime</v>
       </c>
       <c r="I108">
-        <v>100</v>
+        <v>325</v>
       </c>
       <c r="J108">
-        <v>10000</v>
+        <v>32000</v>
       </c>
       <c r="K108" s="1">
         <v>69</v>
@@ -7098,21 +7098,21 @@
       </c>
       <c r="F109" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F109" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>Despicable!</v>
       </c>
       <c r="G109" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G109" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="H109" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H109" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>AskingForIt</v>
       </c>
       <c r="I109">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J109">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K109" s="1">
         <v>50</v>
@@ -7142,21 +7142,21 @@
       </c>
       <c r="F110" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F110" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="G110" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G110" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>MadeIt</v>
       </c>
       <c r="H110" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H110" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="I110">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J110">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K110" s="1">
         <v>134</v>
@@ -7186,21 +7186,21 @@
       </c>
       <c r="F111" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F111" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>ThankGod</v>
       </c>
       <c r="G111" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G111" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>MadeIt</v>
       </c>
       <c r="H111" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H111" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>BackToUs</v>
       </c>
       <c r="I111">
         <v>100</v>
       </c>
       <c r="J111">
-        <v>10000</v>
+        <v>14000</v>
       </c>
       <c r="K111" s="1">
         <v>78</v>
@@ -7230,21 +7230,21 @@
       </c>
       <c r="F112" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F112" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>Drained</v>
       </c>
       <c r="G112" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G112" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>God'sPlan</v>
       </c>
       <c r="H112" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H112" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
         <v>WeLostThem</v>
       </c>
       <c r="I112">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J112">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K112" s="1">
         <v>145</v>
@@ -7274,7 +7274,7 @@
       </c>
       <c r="F113" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F113" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="G113" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G113" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -7282,13 +7282,13 @@
       </c>
       <c r="H113" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H113" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HELPME</v>
+        <v>HardTimes</v>
       </c>
       <c r="I113">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J113">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K113" s="1">
         <v>82</v>
@@ -7322,17 +7322,17 @@
       </c>
       <c r="G114" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G114" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="H114" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H114" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="I114">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="J114">
-        <v>10000</v>
+        <v>26000</v>
       </c>
       <c r="K114" s="1">
         <v>175</v>
@@ -7362,21 +7362,21 @@
       </c>
       <c r="F115" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F115" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="G115" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G115" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="H115" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H115" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
         <v>OverpaidIdiots</v>
       </c>
       <c r="I115">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="J115">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K115" s="1">
         <v>91</v>
@@ -7406,21 +7406,21 @@
       </c>
       <c r="F116" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F116" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="G116" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G116" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>WEStrong</v>
       </c>
       <c r="H116" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H116" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
         <v>CommunityBuild</v>
       </c>
       <c r="I116">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J116">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K116" s="1">
         <v>150</v>
@@ -7454,17 +7454,17 @@
       </c>
       <c r="G117" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G117" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>WEStrong</v>
       </c>
       <c r="H117" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H117" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>WEStrong</v>
       </c>
       <c r="I117">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J117">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K117" s="1">
         <v>110</v>
@@ -7498,17 +7498,17 @@
       </c>
       <c r="G118" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G118" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="H118" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H118" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>Outcast</v>
       </c>
       <c r="I118">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J118">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K118" s="1">
         <v>60</v>
@@ -7538,21 +7538,21 @@
       </c>
       <c r="F119" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F119" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="G119" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G119" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="H119" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H119" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>Desperate</v>
       </c>
       <c r="I119">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J119">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K119" s="1">
         <v>70</v>
@@ -7586,17 +7586,17 @@
       </c>
       <c r="G120" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G120" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="H120" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H120" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="I120">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="J120">
-        <v>10000</v>
+        <v>31000</v>
       </c>
       <c r="K120" s="1">
         <v>147</v>
@@ -7626,21 +7626,21 @@
       </c>
       <c r="F121" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F121" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="G121" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G121" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="H121" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H121" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
         <v>OurLastHope</v>
       </c>
       <c r="I121">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J121">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K121" s="1">
         <v>90</v>
@@ -7670,21 +7670,21 @@
       </c>
       <c r="F122" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F122" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>KeepThemIN!</v>
+        <v>RepeatElection</v>
       </c>
       <c r="G122" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G122" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v>RepeatElection</v>
       </c>
       <c r="H122" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H122" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="I122">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J122">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K122" s="1">
         <v>100</v>
@@ -7718,17 +7718,17 @@
       </c>
       <c r="G123" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G123" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="H123" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H123" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>KeepThemIN!</v>
+        <v>ReElect!!!</v>
       </c>
       <c r="I123">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J123">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K123" s="1">
         <v>156</v>
@@ -7762,17 +7762,17 @@
       </c>
       <c r="G124" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G124" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="H124" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H124" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>I'maSitDown</v>
       </c>
       <c r="I124">
         <v>100</v>
       </c>
       <c r="J124">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K124" s="1">
         <v>80</v>
@@ -7813,10 +7813,10 @@
         <v>NoFaith</v>
       </c>
       <c r="I125">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J125">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K125" s="1">
         <v>75</v>
@@ -7846,7 +7846,7 @@
       </c>
       <c r="F126" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F126" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="G126" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G126" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -7854,13 +7854,13 @@
       </c>
       <c r="H126" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H126" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>CoupDeTahhh</v>
+        <v>ToTheTorches!</v>
       </c>
       <c r="I126">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J126">
-        <v>10000</v>
+        <v>30000</v>
       </c>
       <c r="K126" s="1">
         <v>121</v>
@@ -7894,17 +7894,17 @@
       </c>
       <c r="G127" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G127" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="H127" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H127" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>BurnItDOWN</v>
       </c>
       <c r="I127">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J127">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K127" s="1">
         <v>131</v>
@@ -7934,7 +7934,7 @@
       </c>
       <c r="F128" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F128" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="G128" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G128" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -7942,10 +7942,10 @@
       </c>
       <c r="H128" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H128" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>StrongerTogether</v>
       </c>
       <c r="I128">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J128">
         <v>10000</v>
@@ -7978,21 +7978,21 @@
       </c>
       <c r="F129" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F129" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>Hero</v>
       </c>
       <c r="G129" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G129" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>Justice</v>
       </c>
       <c r="H129" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H129" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>Justified!</v>
       </c>
       <c r="I129">
         <v>100</v>
       </c>
       <c r="J129">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K129" s="1">
         <v>132</v>
@@ -8022,7 +8022,7 @@
       </c>
       <c r="F130" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F130" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>SoTragic</v>
       </c>
       <c r="G130" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G130" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -8030,13 +8030,13 @@
       </c>
       <c r="H130" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H130" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>TooSoon</v>
       </c>
       <c r="I130">
-        <v>100</v>
+        <v>225</v>
       </c>
       <c r="J130">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K130" s="1">
         <v>149</v>
@@ -8070,17 +8070,17 @@
       </c>
       <c r="G131" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G131" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FreeThem</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="H131" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H131" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FreeThem</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="I131">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J131">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K131" s="1">
         <v>89</v>
@@ -8110,21 +8110,21 @@
       </c>
       <c r="F132" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F132" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>AskingForIt</v>
       </c>
       <c r="G132" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G132" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>DeathCollection</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="H132" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H132" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="I132">
-        <v>100</v>
+        <v>325</v>
       </c>
       <c r="J132">
-        <v>10000</v>
+        <v>32000</v>
       </c>
       <c r="K132" s="1">
         <v>69</v>
@@ -8154,21 +8154,21 @@
       </c>
       <c r="F133" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F133" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>AskingForIt</v>
       </c>
       <c r="G133" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G133" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>PaybackTime</v>
       </c>
       <c r="H133" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H133" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>PaybackTime</v>
       </c>
       <c r="I133">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J133">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K133" s="1">
         <v>50</v>
@@ -8198,7 +8198,7 @@
       </c>
       <c r="F134" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F134" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>BackToUs</v>
       </c>
       <c r="G134" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G134" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -8206,13 +8206,13 @@
       </c>
       <c r="H134" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H134" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="I134">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J134">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K134" s="1">
         <v>134</v>
@@ -8242,21 +8242,21 @@
       </c>
       <c r="F135" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F135" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>MadeIt</v>
       </c>
       <c r="G135" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G135" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Hugs&amp;Kisses</v>
+        <v>MadeIt</v>
       </c>
       <c r="H135" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H135" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>BackToUs</v>
       </c>
       <c r="I135">
         <v>100</v>
       </c>
       <c r="J135">
-        <v>10000</v>
+        <v>14000</v>
       </c>
       <c r="K135" s="1">
         <v>78</v>
@@ -8286,7 +8286,7 @@
       </c>
       <c r="F136" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F136" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>HELPME</v>
       </c>
       <c r="G136" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G136" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -8294,13 +8294,13 @@
       </c>
       <c r="H136" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H136" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Depressing</v>
+        <v>WeLostThem</v>
       </c>
       <c r="I136">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J136">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K136" s="1">
         <v>145</v>
@@ -8330,21 +8330,21 @@
       </c>
       <c r="F137" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F137" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>I'mSoLost</v>
       </c>
       <c r="G137" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G137" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>Drained</v>
       </c>
       <c r="H137" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H137" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>HELPME</v>
       </c>
       <c r="I137">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J137">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K137" s="1">
         <v>82</v>
@@ -8374,21 +8374,21 @@
       </c>
       <c r="F138" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F138" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>CrapStaff</v>
       </c>
       <c r="G138" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G138" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="H138" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H138" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>Refund</v>
       </c>
       <c r="I138">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="J138">
-        <v>10000</v>
+        <v>26000</v>
       </c>
       <c r="K138" s="1">
         <v>175</v>
@@ -8418,21 +8418,21 @@
       </c>
       <c r="F139" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F139" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>LONGWaitTimes</v>
       </c>
       <c r="G139" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G139" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="H139" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H139" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="I139">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="J139">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K139" s="1">
         <v>91</v>
@@ -8462,21 +8462,21 @@
       </c>
       <c r="F140" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F140" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>WEStrong</v>
       </c>
       <c r="G140" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G140" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="H140" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H140" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="I140">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J140">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K140" s="1">
         <v>150</v>
@@ -8506,21 +8506,21 @@
       </c>
       <c r="F141" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F141" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="G141" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G141" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>WEStrong</v>
       </c>
       <c r="H141" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H141" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>WEStrong</v>
       </c>
       <c r="I141">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J141">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K141" s="1">
         <v>110</v>
@@ -8550,21 +8550,21 @@
       </c>
       <c r="F142" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F142" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="G142" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G142" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="H142" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H142" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WeNeedChange</v>
+        <v>Outcast</v>
       </c>
       <c r="I142">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J142">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K142" s="1">
         <v>60</v>
@@ -8594,21 +8594,21 @@
       </c>
       <c r="F143" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F143" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>SplitUp</v>
       </c>
       <c r="G143" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G143" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>Desperate</v>
       </c>
       <c r="H143" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H143" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>SplitUp</v>
       </c>
       <c r="I143">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J143">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K143" s="1">
         <v>70</v>
@@ -8642,17 +8642,17 @@
       </c>
       <c r="G144" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G144" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="H144" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H144" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>NecessaryEvil</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="I144">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="J144">
-        <v>10000</v>
+        <v>31000</v>
       </c>
       <c r="K144" s="1">
         <v>147</v>
@@ -8682,21 +8682,21 @@
       </c>
       <c r="F145" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F145" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>NecessaryEvil</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="G145" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G145" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>Messiah</v>
       </c>
       <c r="H145" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H145" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
         <v>Messiah</v>
       </c>
       <c r="I145">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J145">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K145" s="1">
         <v>90</v>
@@ -8730,17 +8730,17 @@
       </c>
       <c r="G146" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G146" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v>RepeatElection</v>
       </c>
       <c r="H146" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H146" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v xml:space="preserve">Saviours </v>
       </c>
       <c r="I146">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J146">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K146" s="1">
         <v>100</v>
@@ -8774,17 +8774,17 @@
       </c>
       <c r="G147" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G147" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="H147" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H147" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>People'sVoice</v>
       </c>
       <c r="I147">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J147">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K147" s="1">
         <v>156</v>
@@ -8814,11 +8814,11 @@
       </c>
       <c r="F148" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F148" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>ItsOver</v>
       </c>
       <c r="G148" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G148" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>NoFaith</v>
       </c>
       <c r="H148" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H148" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -8828,7 +8828,7 @@
         <v>100</v>
       </c>
       <c r="J148">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K148" s="1">
         <v>80</v>
@@ -8858,21 +8858,21 @@
       </c>
       <c r="F149" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F149" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>ItsOver</v>
       </c>
       <c r="G149" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G149" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>ItsOver</v>
       </c>
       <c r="H149" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H149" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
         <v>ItsOver</v>
       </c>
       <c r="I149">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J149">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K149" s="1">
         <v>75</v>
@@ -8902,21 +8902,21 @@
       </c>
       <c r="F150" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F150" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="G150" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G150" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RiotTIME</v>
+        <v>RaidingNight</v>
       </c>
       <c r="H150" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H150" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
         <v>RaidingNight</v>
       </c>
       <c r="I150">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J150">
-        <v>10000</v>
+        <v>30000</v>
       </c>
       <c r="K150" s="1">
         <v>121</v>
@@ -8946,7 +8946,7 @@
       </c>
       <c r="F151" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F151" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>RiotTIME</v>
       </c>
       <c r="G151" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G151" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -8954,13 +8954,13 @@
       </c>
       <c r="H151" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H151" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>BurnItDOWN</v>
       </c>
       <c r="I151">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J151">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K151" s="1">
         <v>131</v>
@@ -8990,18 +8990,18 @@
       </c>
       <c r="F152" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F152" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="G152" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G152" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>ComeTogether!!</v>
       </c>
       <c r="H152" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H152" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>StrongerTogether</v>
       </c>
       <c r="I152">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J152">
         <v>10000</v>
@@ -9034,21 +9034,21 @@
       </c>
       <c r="F153" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F153" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>ComeTogether!!</v>
       </c>
       <c r="G153" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G153" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>Justice</v>
       </c>
       <c r="H153" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H153" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>Justified!</v>
       </c>
       <c r="I153">
         <v>100</v>
       </c>
       <c r="J153">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K153" s="1">
         <v>132</v>
@@ -9078,21 +9078,21 @@
       </c>
       <c r="F154" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F154" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>WhatAShame</v>
       </c>
       <c r="G154" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G154" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>FreeThem</v>
       </c>
       <c r="H154" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H154" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="I154">
-        <v>100</v>
+        <v>225</v>
       </c>
       <c r="J154">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K154" s="1">
         <v>149</v>
@@ -9122,7 +9122,7 @@
       </c>
       <c r="F155" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F155" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="G155" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G155" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -9130,13 +9130,13 @@
       </c>
       <c r="H155" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H155" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>Lowlife</v>
       </c>
       <c r="I155">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J155">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K155" s="1">
         <v>89</v>
@@ -9166,21 +9166,21 @@
       </c>
       <c r="F156" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F156" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>Despicable!</v>
       </c>
       <c r="G156" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G156" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>Despicable!</v>
       </c>
       <c r="H156" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H156" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
         <v>Despicable!</v>
       </c>
       <c r="I156">
-        <v>100</v>
+        <v>325</v>
       </c>
       <c r="J156">
-        <v>10000</v>
+        <v>32000</v>
       </c>
       <c r="K156" s="1">
         <v>69</v>
@@ -9210,21 +9210,21 @@
       </c>
       <c r="F157" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F157" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="G157" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G157" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="H157" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H157" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>DeathCollection</v>
+        <v>Despicable!</v>
       </c>
       <c r="I157">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J157">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K157" s="1">
         <v>50</v>
@@ -9254,21 +9254,21 @@
       </c>
       <c r="F158" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F158" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>ThankGod</v>
       </c>
       <c r="G158" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G158" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>100Sober</v>
+        <v>MadeIt</v>
       </c>
       <c r="H158" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H158" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>BestWishes</v>
       </c>
       <c r="I158">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J158">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K158" s="1">
         <v>134</v>
@@ -9298,21 +9298,21 @@
       </c>
       <c r="F159" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F159" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>100Sober</v>
       </c>
       <c r="G159" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G159" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>100Sober</v>
       </c>
       <c r="H159" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H159" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="I159">
         <v>100</v>
       </c>
       <c r="J159">
-        <v>10000</v>
+        <v>14000</v>
       </c>
       <c r="K159" s="1">
         <v>78</v>
@@ -9342,7 +9342,7 @@
       </c>
       <c r="F160" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F160" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Depressing</v>
+        <v>God'sPlan</v>
       </c>
       <c r="G160" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G160" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -9350,13 +9350,13 @@
       </c>
       <c r="H160" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H160" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>Depressing</v>
       </c>
       <c r="I160">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J160">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K160" s="1">
         <v>145</v>
@@ -9386,21 +9386,21 @@
       </c>
       <c r="F161" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F161" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="G161" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G161" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="H161" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H161" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
         <v>HardTimes</v>
       </c>
       <c r="I161">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J161">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K161" s="1">
         <v>82</v>
@@ -9430,21 +9430,21 @@
       </c>
       <c r="F162" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F162" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="G162" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G162" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="H162" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H162" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>Refund</v>
       </c>
       <c r="I162">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="J162">
-        <v>10000</v>
+        <v>26000</v>
       </c>
       <c r="K162" s="1">
         <v>175</v>
@@ -9474,21 +9474,21 @@
       </c>
       <c r="F163" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F163" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>LONGWaitTimes</v>
       </c>
       <c r="G163" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G163" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>CrapStaff</v>
       </c>
       <c r="H163" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H163" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>CrapStaff</v>
       </c>
       <c r="I163">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="J163">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K163" s="1">
         <v>91</v>
@@ -9522,17 +9522,17 @@
       </c>
       <c r="G164" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G164" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="H164" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H164" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>ALWAYSSupport</v>
       </c>
       <c r="I164">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J164">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K164" s="1">
         <v>150</v>
@@ -9562,21 +9562,21 @@
       </c>
       <c r="F165" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F165" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="G165" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G165" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="H165" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H165" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
         <v>OurWayOrHiWay</v>
       </c>
       <c r="I165">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J165">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K165" s="1">
         <v>110</v>
@@ -9606,21 +9606,21 @@
       </c>
       <c r="F166" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F166" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>SplitUp</v>
       </c>
       <c r="G166" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G166" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="H166" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H166" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>Outcast</v>
       </c>
       <c r="I166">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J166">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K166" s="1">
         <v>60</v>
@@ -9654,17 +9654,17 @@
       </c>
       <c r="G167" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G167" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="H167" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H167" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="I167">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J167">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K167" s="1">
         <v>70</v>
@@ -9698,17 +9698,17 @@
       </c>
       <c r="G168" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G168" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>Messiah</v>
       </c>
       <c r="H168" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H168" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>OurLastHope</v>
       </c>
       <c r="I168">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="J168">
-        <v>10000</v>
+        <v>31000</v>
       </c>
       <c r="K168" s="1">
         <v>147</v>
@@ -9738,21 +9738,21 @@
       </c>
       <c r="F169" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F169" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="G169" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G169" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="H169" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H169" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
         <v>Divide&amp;CONQUER</v>
       </c>
       <c r="I169">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J169">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K169" s="1">
         <v>90</v>
@@ -9782,21 +9782,21 @@
       </c>
       <c r="F170" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F170" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="G170" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G170" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>People'sVoice</v>
       </c>
       <c r="H170" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H170" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>People'sVoice</v>
+        <v>InGoodHands</v>
       </c>
       <c r="I170">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J170">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K170" s="1">
         <v>100</v>
@@ -9826,21 +9826,21 @@
       </c>
       <c r="F171" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F171" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>People'sVoice</v>
+        <v>InGoodHands</v>
       </c>
       <c r="G171" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G171" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>InGoodHands</v>
       </c>
       <c r="H171" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H171" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>InGoodHands</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="I171">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J171">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K171" s="1">
         <v>156</v>
@@ -9870,21 +9870,21 @@
       </c>
       <c r="F172" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F172" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>WhatAJoke</v>
       </c>
       <c r="G172" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G172" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>NoFaith</v>
       </c>
       <c r="H172" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H172" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>WhatAJoke</v>
       </c>
       <c r="I172">
         <v>100</v>
       </c>
       <c r="J172">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K172" s="1">
         <v>80</v>
@@ -9914,21 +9914,21 @@
       </c>
       <c r="F173" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F173" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>NoFaith</v>
       </c>
       <c r="G173" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G173" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="H173" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H173" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NoFaith</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="I173">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J173">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K173" s="1">
         <v>75</v>
@@ -9958,7 +9958,7 @@
       </c>
       <c r="F174" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F174" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RiotTIME</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="G174" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G174" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -9966,13 +9966,13 @@
       </c>
       <c r="H174" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H174" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="I174">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J174">
-        <v>10000</v>
+        <v>30000</v>
       </c>
       <c r="K174" s="1">
         <v>121</v>
@@ -10002,21 +10002,21 @@
       </c>
       <c r="F175" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F175" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>CoupDeTahhh</v>
+        <v>RaidingNight</v>
       </c>
       <c r="G175" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G175" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>CoupDeTahhh</v>
+        <v>RaidingNight</v>
       </c>
       <c r="H175" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H175" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="I175">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J175">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K175" s="1">
         <v>131</v>
@@ -10046,7 +10046,7 @@
       </c>
       <c r="F176" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F176" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>BeSafe</v>
       </c>
       <c r="G176" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G176" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -10054,10 +10054,10 @@
       </c>
       <c r="H176" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H176" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>Justice</v>
       </c>
       <c r="I176">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J176">
         <v>10000</v>
@@ -10090,7 +10090,7 @@
       </c>
       <c r="F177" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F177" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="G177" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G177" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -10098,13 +10098,13 @@
       </c>
       <c r="H177" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H177" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>Justice</v>
       </c>
       <c r="I177">
         <v>100</v>
       </c>
       <c r="J177">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K177" s="1">
         <v>132</v>
@@ -10134,21 +10134,21 @@
       </c>
       <c r="F178" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F178" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>Lowlife</v>
       </c>
       <c r="G178" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G178" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>PrayForThem</v>
       </c>
       <c r="H178" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H178" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>SoTragic</v>
       </c>
       <c r="I178">
-        <v>100</v>
+        <v>225</v>
       </c>
       <c r="J178">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K178" s="1">
         <v>149</v>
@@ -10182,17 +10182,17 @@
       </c>
       <c r="G179" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G179" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>SoTragic</v>
       </c>
       <c r="H179" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H179" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>PrayForThem</v>
       </c>
       <c r="I179">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J179">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K179" s="1">
         <v>89</v>
@@ -10222,21 +10222,21 @@
       </c>
       <c r="F180" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F180" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>PaybackTime</v>
       </c>
       <c r="G180" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G180" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="H180" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H180" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="I180">
-        <v>100</v>
+        <v>325</v>
       </c>
       <c r="J180">
-        <v>10000</v>
+        <v>32000</v>
       </c>
       <c r="K180" s="1">
         <v>69</v>
@@ -10266,21 +10266,21 @@
       </c>
       <c r="F181" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F181" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="G181" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G181" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="H181" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H181" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>AskingForIt</v>
       </c>
       <c r="I181">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J181">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K181" s="1">
         <v>50</v>
@@ -10310,7 +10310,7 @@
       </c>
       <c r="F182" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F182" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="G182" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G182" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -10318,13 +10318,13 @@
       </c>
       <c r="H182" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H182" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>100Sober</v>
+        <v>ThankGod</v>
       </c>
       <c r="I182">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J182">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="K182" s="1">
         <v>134</v>
@@ -10354,21 +10354,21 @@
       </c>
       <c r="F183" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F183" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>100Sober</v>
+        <v>BackToUs</v>
       </c>
       <c r="G183" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G183" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="H183" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H183" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>BestWishes</v>
       </c>
       <c r="I183">
         <v>100</v>
       </c>
       <c r="J183">
-        <v>10000</v>
+        <v>14000</v>
       </c>
       <c r="K183" s="1">
         <v>78</v>
@@ -10398,21 +10398,21 @@
       </c>
       <c r="F184" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F184" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="G184" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G184" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>Drained</v>
       </c>
       <c r="H184" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H184" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Depressing</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="I184">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J184">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K184" s="1">
         <v>145</v>
@@ -10442,21 +10442,21 @@
       </c>
       <c r="F185" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F185" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Depressing</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="G185" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G185" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>HardTimes</v>
       </c>
       <c r="H185" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H185" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="I185">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J185">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K185" s="1">
         <v>82</v>
@@ -10490,17 +10490,17 @@
       </c>
       <c r="G186" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G186" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="H186" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H186" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="I186">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="J186">
-        <v>10000</v>
+        <v>26000</v>
       </c>
       <c r="K186" s="1">
         <v>175</v>
@@ -10530,21 +10530,21 @@
       </c>
       <c r="F187" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F187" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="G187" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G187" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>Refund</v>
       </c>
       <c r="H187" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H187" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>Refund</v>
       </c>
       <c r="I187">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="J187">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K187" s="1">
         <v>91</v>
@@ -10574,21 +10574,21 @@
       </c>
       <c r="F188" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F188" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="G188" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G188" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>WEStrong</v>
       </c>
       <c r="H188" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H188" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>ALWAYSSupport</v>
       </c>
       <c r="I188">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J188">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="K188" s="1">
         <v>150</v>
@@ -10618,21 +10618,21 @@
       </c>
       <c r="F189" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F189" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="G189" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G189" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="H189" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H189" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="I189">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J189">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="K189" s="1">
         <v>110</v>
@@ -10666,17 +10666,17 @@
       </c>
       <c r="G190" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G190" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="H190" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H190" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>SplitUp</v>
       </c>
       <c r="I190">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J190">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K190" s="1">
         <v>60</v>
@@ -10706,21 +10706,21 @@
       </c>
       <c r="F191" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F191" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="G191" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G191" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>Desperate</v>
       </c>
       <c r="H191" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H191" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>SplitUp</v>
       </c>
       <c r="I191">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J191">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="K191" s="1">
         <v>70</v>
@@ -10750,7 +10750,7 @@
       </c>
       <c r="F192" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F192" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="G192" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G192" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -10758,13 +10758,13 @@
       </c>
       <c r="H192" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H192" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="I192">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="J192">
-        <v>10000</v>
+        <v>31000</v>
       </c>
       <c r="K192" s="1">
         <v>147</v>
@@ -10794,21 +10794,21 @@
       </c>
       <c r="F193" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F193" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="G193" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G193" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="H193" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H193" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>NecessaryEvil</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="I193">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J193">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K193" s="1">
         <v>90</v>
@@ -13576,7 +13576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53B4979-BA2F-42C6-BF9E-77AF10AFAE50}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor edit to text messages
</commit_message>
<xml_diff>
--- a/Source/Narrative/Game Data.xlsx
+++ b/Source/Narrative/Game Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtsp1\Documents\GitHub\The-Cool-Guys\UnderChoices\Source\Narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90EDA76-1127-4812-BB93-735F62D6325C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CD27FA-7CC0-4A9F-9DCB-A7B89C2568BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Media Posts" sheetId="1" r:id="rId1"/>
@@ -1440,9 +1440,6 @@
     <t>Heyo Moleque; I know you're busy; but I need a ride to an apointment with the doc.|Nothing serious; just a check up. Apointment's tomorrow; just before you get on the clock.|I hope it's not too much trouble. I'll see you then.</t>
   </si>
   <si>
-    <t>Heyo there Moleque! Still at the doctor's office.|They're saying I'm fine; but they wanna have me back in in a few days for some blood tests.|Don't worry; they say it's just to make sure I'm in tip top shape. Loves ya!</t>
-  </si>
-  <si>
     <t>Heyo Moleque! You been seeing this crazy stuff about that new flu they're talking about?|Got my neighbours going nuts about locking up the house. I told em that I am confident the govs got it all locked up.|Either way Moleque; hope you're staying safe and healthy!</t>
   </si>
   <si>
@@ -1786,6 +1783,9 @@
   </si>
   <si>
     <t>Pigeons</t>
+  </si>
+  <si>
+    <t>Heyo there Moleque! Still at the doctor's office.|This stuff that's been posted lately is real depressing lately, so I'm hoping I'll get to see ya soon.|The doctor is saying I'm fine; but they wanna have me back in in a few days for some blood tests.|Don't worry; they say it's just to make sure I'm in tip top shape. Loves ya!</t>
   </si>
 </sst>
 </file>
@@ -2338,7 +2338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -2369,7 +2369,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -2417,11 +2417,11 @@
       </c>
       <c r="F2" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F2" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>RepeatElection</v>
       </c>
       <c r="G2" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G2" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>KeepThemIN!</v>
+        <v>RepeatElection</v>
       </c>
       <c r="H2" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H2" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -2437,7 +2437,7 @@
         <v>150</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="M2" s="19" t="s">
         <v>233</v>
@@ -2461,15 +2461,15 @@
       </c>
       <c r="F3" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F3" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>KeepThemIN!</v>
+        <v>VoteAgain</v>
       </c>
       <c r="G3" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G3" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>ReElect!!!</v>
       </c>
       <c r="H3" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H3" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v xml:space="preserve">Saviours </v>
       </c>
       <c r="I3">
         <v>50</v>
@@ -2481,7 +2481,7 @@
         <v>150</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="M3" s="19" t="s">
         <v>239</v>
@@ -2505,15 +2505,15 @@
       </c>
       <c r="F4" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F4" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>ItsOver</v>
       </c>
       <c r="G4" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G4" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="H4" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H4" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="I4">
         <v>100</v>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="F5" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F5" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>ItsOver</v>
       </c>
       <c r="G5" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G5" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="H5" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H5" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="I5">
         <v>125</v>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="F6" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F6" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>RiotTIME</v>
       </c>
       <c r="G6" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="H6" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H6" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="I6">
         <v>200</v>
@@ -2637,15 +2637,15 @@
       </c>
       <c r="F7" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F7" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>ToTheTorches!</v>
       </c>
       <c r="G7" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G7" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RiotTIME</v>
+        <v>ToTheTorches!</v>
       </c>
       <c r="H7" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="I7">
         <v>125</v>
@@ -2660,7 +2660,7 @@
         <v>96</v>
       </c>
       <c r="M7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2681,15 +2681,15 @@
       </c>
       <c r="F8" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F8" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="G8" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G8" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FightBackTeam!</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="H8" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H8" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="I8">
         <v>75</v>
@@ -2704,7 +2704,7 @@
         <v>97</v>
       </c>
       <c r="M8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2725,15 +2725,15 @@
       </c>
       <c r="F9" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F9" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>Justice</v>
       </c>
       <c r="G9" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G9" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="H9" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H9" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>Justified!</v>
       </c>
       <c r="I9">
         <v>100</v>
@@ -2748,7 +2748,7 @@
         <v>98</v>
       </c>
       <c r="M9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2769,15 +2769,15 @@
       </c>
       <c r="F10" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>Pathetic</v>
       </c>
       <c r="G10" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G10" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>WhatAShame</v>
       </c>
       <c r="H10" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H10" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="I10">
         <v>225</v>
@@ -2792,7 +2792,7 @@
         <v>99</v>
       </c>
       <c r="M10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2813,15 +2813,15 @@
       </c>
       <c r="F11" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>Lowlife</v>
       </c>
       <c r="G11" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G11" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>PrayForThem</v>
       </c>
       <c r="H11" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H11" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>FreeThem</v>
       </c>
       <c r="I11">
         <v>175</v>
@@ -2836,7 +2836,7 @@
         <v>100</v>
       </c>
       <c r="M11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2857,14 +2857,14 @@
       </c>
       <c r="F12" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>Despicable!</v>
       </c>
       <c r="G12" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G12" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I12">
         <v>325</v>
@@ -2900,15 +2900,15 @@
       </c>
       <c r="F13" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>DeathCollection</v>
       </c>
       <c r="G13" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G13" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>AskingForIt</v>
       </c>
       <c r="H13" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H13" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="I13">
         <v>200</v>
@@ -2948,11 +2948,11 @@
       </c>
       <c r="G14" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G14" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>ThankGod</v>
       </c>
       <c r="H14" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H14" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>BestWishes</v>
       </c>
       <c r="I14">
         <v>75</v>
@@ -2988,15 +2988,15 @@
       </c>
       <c r="F15" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F15" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="G15" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G15" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>ThankGod</v>
       </c>
       <c r="H15" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H15" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>Recovered:)</v>
       </c>
       <c r="I15">
         <v>100</v>
@@ -3032,15 +3032,15 @@
       </c>
       <c r="F16" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F16" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>WeLostThem</v>
       </c>
       <c r="G16" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>God'sPlan</v>
       </c>
       <c r="H16" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H16" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>God'sPlan</v>
       </c>
       <c r="I16">
         <v>200</v>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="F17" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F17" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HELPME</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="G17" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G17" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -3084,7 +3084,7 @@
       </c>
       <c r="H17" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H17" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="I17">
         <v>175</v>
@@ -3120,15 +3120,15 @@
       </c>
       <c r="F18" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F18" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="G18" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="H18" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H18" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="I18">
         <v>350</v>
@@ -3164,15 +3164,15 @@
       </c>
       <c r="F19" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F19" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>CrapStaff</v>
       </c>
       <c r="G19" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="H19" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H19" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>Refund</v>
       </c>
       <c r="I19">
         <v>250</v>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="F20" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F20" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="G20" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -3216,7 +3216,7 @@
       </c>
       <c r="H20" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H20" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="I20">
         <v>75</v>
@@ -3256,11 +3256,11 @@
       </c>
       <c r="G21" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>WEStrong</v>
       </c>
       <c r="H21" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H21" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="I21">
         <v>50</v>
@@ -3296,15 +3296,15 @@
       </c>
       <c r="F22" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F22" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="G22" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="H22" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H22" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="I22">
         <v>150</v>
@@ -3344,7 +3344,7 @@
       </c>
       <c r="G23" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="H23" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H23" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -3384,7 +3384,7 @@
       </c>
       <c r="F24" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F24" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>OurLastHope</v>
       </c>
       <c r="G24" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G24" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -3392,7 +3392,7 @@
       </c>
       <c r="H24" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H24" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>OurLastHope</v>
       </c>
       <c r="I24">
         <v>400</v>
@@ -3428,15 +3428,15 @@
       </c>
       <c r="F25" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F25" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="G25" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G25" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>Messiah</v>
       </c>
       <c r="H25" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H25" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="I25">
         <v>150</v>
@@ -3472,11 +3472,11 @@
       </c>
       <c r="F26" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F26" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="G26" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G26" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>InGoodHands</v>
+        <v>People'sVoice</v>
       </c>
       <c r="H26" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H26" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -3492,7 +3492,7 @@
         <v>150</v>
       </c>
       <c r="L26" s="19" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="M26" s="19" t="s">
         <v>233</v>
@@ -3516,15 +3516,15 @@
       </c>
       <c r="F27" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F27" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>InGoodHands</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="G27" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G27" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v>InGoodHands</v>
       </c>
       <c r="H27" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H27" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="I27">
         <v>50</v>
@@ -3536,7 +3536,7 @@
         <v>150</v>
       </c>
       <c r="L27" s="20" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="M27" s="19" t="s">
         <v>239</v>
@@ -3560,15 +3560,15 @@
       </c>
       <c r="F28" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F28" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="G28" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G28" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>NoFaith</v>
       </c>
       <c r="H28" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H28" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>ItsOver</v>
       </c>
       <c r="I28">
         <v>100</v>
@@ -3604,15 +3604,15 @@
       </c>
       <c r="F29" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F29" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="G29" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G29" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="H29" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H29" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>NoFaith</v>
       </c>
       <c r="I29">
         <v>125</v>
@@ -3648,15 +3648,15 @@
       </c>
       <c r="F30" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F30" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>BurnItDOWN</v>
       </c>
       <c r="G30" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G30" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>CoupDeTahhh</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="H30" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H30" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>ToTheTorches!</v>
       </c>
       <c r="I30">
         <v>200</v>
@@ -3692,15 +3692,15 @@
       </c>
       <c r="F31" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F31" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="G31" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G31" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="H31" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H31" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="I31">
         <v>125</v>
@@ -3715,7 +3715,7 @@
         <v>96</v>
       </c>
       <c r="M31" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -3740,11 +3740,11 @@
       </c>
       <c r="G32" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G32" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>Justice</v>
       </c>
       <c r="H32" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H32" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>Justified!</v>
       </c>
       <c r="I32">
         <v>75</v>
@@ -3759,7 +3759,7 @@
         <v>97</v>
       </c>
       <c r="M32" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -3780,15 +3780,15 @@
       </c>
       <c r="F33" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F33" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="G33" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G33" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>StrongerTogether</v>
       </c>
       <c r="H33" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H33" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="I33">
         <v>100</v>
@@ -3803,7 +3803,7 @@
         <v>98</v>
       </c>
       <c r="M33" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -3824,11 +3824,11 @@
       </c>
       <c r="F34" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F34" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>Lowlife</v>
       </c>
       <c r="G34" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G34" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FreeThem</v>
+        <v>SoTragic</v>
       </c>
       <c r="H34" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H34" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -3847,7 +3847,7 @@
         <v>99</v>
       </c>
       <c r="M34" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -3868,15 +3868,15 @@
       </c>
       <c r="F35" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F35" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="G35" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G35" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>SoTragic</v>
       </c>
       <c r="H35" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H35" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>Pathetic</v>
       </c>
       <c r="I35">
         <v>175</v>
@@ -3891,7 +3891,7 @@
         <v>100</v>
       </c>
       <c r="M35" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -3916,11 +3916,11 @@
       </c>
       <c r="G36" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G36" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="H36" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H36" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>DeathCollection</v>
       </c>
       <c r="I36">
         <v>325</v>
@@ -3956,15 +3956,15 @@
       </c>
       <c r="F37" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F37" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="G37" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G37" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="H37" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H37" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>PaybackTime</v>
       </c>
       <c r="I37">
         <v>200</v>
@@ -4000,15 +4000,15 @@
       </c>
       <c r="F38" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F38" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>ThankGod</v>
       </c>
       <c r="G38" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G38" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>MadeIt</v>
       </c>
       <c r="H38" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H38" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>BackToUs</v>
       </c>
       <c r="I38">
         <v>75</v>
@@ -4044,7 +4044,7 @@
       </c>
       <c r="F39" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F39" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="G39" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G39" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="H39" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H39" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>Recovered:)</v>
       </c>
       <c r="I39">
         <v>100</v>
@@ -4088,15 +4088,15 @@
       </c>
       <c r="F40" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F40" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>Drained</v>
       </c>
       <c r="G40" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G40" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HELPME</v>
+        <v>Depressing</v>
       </c>
       <c r="H40" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H40" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>Depressing</v>
       </c>
       <c r="I40">
         <v>200</v>
@@ -4132,15 +4132,15 @@
       </c>
       <c r="F41" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F41" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HELPME</v>
+        <v>I'mSoLost</v>
       </c>
       <c r="G41" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G41" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>Drained</v>
       </c>
       <c r="H41" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H41" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>Depressing</v>
       </c>
       <c r="I41">
         <v>175</v>
@@ -4176,15 +4176,15 @@
       </c>
       <c r="F42" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F42" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="G42" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G42" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="H42" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H42" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>Refund</v>
       </c>
       <c r="I42">
         <v>350</v>
@@ -4220,15 +4220,15 @@
       </c>
       <c r="F43" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F43" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>Refund</v>
       </c>
       <c r="G43" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G43" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="H43" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H43" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="I43">
         <v>250</v>
@@ -4264,15 +4264,15 @@
       </c>
       <c r="F44" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F44" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="G44" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G44" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="H44" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H44" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WEStrong</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="I44">
         <v>75</v>
@@ -4308,15 +4308,15 @@
       </c>
       <c r="F45" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F45" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>CommunityBuild</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="G45" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G45" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="H45" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H45" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>WEStrong</v>
       </c>
       <c r="I45">
         <v>50</v>
@@ -4352,15 +4352,15 @@
       </c>
       <c r="F46" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F46" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="G46" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G46" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="H46" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H46" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>Desperate</v>
       </c>
       <c r="I46">
         <v>150</v>
@@ -4396,11 +4396,11 @@
       </c>
       <c r="F47" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F47" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="G47" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G47" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="H47" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H47" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -4440,15 +4440,15 @@
       </c>
       <c r="F48" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F48" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="G48" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G48" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="H48" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H48" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="I48">
         <v>400</v>
@@ -4484,15 +4484,15 @@
       </c>
       <c r="F49" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F49" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="G49" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G49" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="H49" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H49" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="I49">
         <v>150</v>
@@ -4528,15 +4528,15 @@
       </c>
       <c r="F50" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F50" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>ReElect!!!</v>
       </c>
       <c r="G50" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G50" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v>VoteAgain</v>
       </c>
       <c r="H50" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H50" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>People'sVoice</v>
+        <v xml:space="preserve">Saviours </v>
       </c>
       <c r="I50">
         <v>75</v>
@@ -4548,7 +4548,7 @@
         <v>150</v>
       </c>
       <c r="L50" s="21" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="M50" s="19" t="s">
         <v>252</v>
@@ -4572,11 +4572,11 @@
       </c>
       <c r="F51" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F51" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>InGoodHands</v>
+        <v>People'sVoice</v>
       </c>
       <c r="G51" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G51" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v>InGoodHands</v>
       </c>
       <c r="H51" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H51" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -4592,7 +4592,7 @@
         <v>150</v>
       </c>
       <c r="L51" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="M51" s="8" t="s">
         <v>253</v>
@@ -4616,15 +4616,15 @@
       </c>
       <c r="F52" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F52" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>ItsOver</v>
       </c>
       <c r="G52" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G52" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>ItsOver</v>
       </c>
       <c r="H52" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H52" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="I52">
         <v>100</v>
@@ -4660,7 +4660,7 @@
       </c>
       <c r="F53" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F53" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>ItsOver</v>
       </c>
       <c r="G53" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G53" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -4668,7 +4668,7 @@
       </c>
       <c r="H53" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H53" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="I53">
         <v>125</v>
@@ -4704,15 +4704,15 @@
       </c>
       <c r="F54" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F54" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="G54" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G54" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>RaidingNight</v>
       </c>
       <c r="H54" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H54" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>RiotTIME</v>
       </c>
       <c r="I54">
         <v>200</v>
@@ -4724,7 +4724,7 @@
         <v>50</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="M54" t="s">
         <v>256</v>
@@ -4748,15 +4748,15 @@
       </c>
       <c r="F55" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F55" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="G55" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G55" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="H55" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H55" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="I55">
         <v>125</v>
@@ -4768,7 +4768,7 @@
         <v>50</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="M55" t="s">
         <v>257</v>
@@ -4792,15 +4792,15 @@
       </c>
       <c r="F56" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F56" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="G56" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G56" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="H56" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H56" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>BeSafe</v>
       </c>
       <c r="I56">
         <v>75</v>
@@ -4836,7 +4836,7 @@
       </c>
       <c r="F57" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F57" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>Justice</v>
       </c>
       <c r="G57" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G57" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="H57" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H57" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="I57">
         <v>100</v>
@@ -4884,11 +4884,11 @@
       </c>
       <c r="G58" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G58" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="H58" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H58" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>FreeThem</v>
       </c>
       <c r="I58">
         <v>225</v>
@@ -4924,15 +4924,15 @@
       </c>
       <c r="F59" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F59" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>PrayForThem</v>
       </c>
       <c r="G59" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G59" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>TooSoon</v>
       </c>
       <c r="H59" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H59" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>WhatAShame</v>
       </c>
       <c r="I59">
         <v>175</v>
@@ -4968,15 +4968,15 @@
       </c>
       <c r="F60" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F60" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>AskingForIt</v>
       </c>
       <c r="G60" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G60" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="H60" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H60" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="I60">
         <v>325</v>
@@ -5016,11 +5016,11 @@
       </c>
       <c r="G61" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G61" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>DeathCollection</v>
       </c>
       <c r="H61" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H61" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>Despicable!</v>
       </c>
       <c r="I61">
         <v>200</v>
@@ -5056,15 +5056,15 @@
       </c>
       <c r="F62" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F62" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>100Sober</v>
+        <v>MadeIt</v>
       </c>
       <c r="G62" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G62" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>MadeIt</v>
       </c>
       <c r="H62" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H62" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>100Sober</v>
       </c>
       <c r="I62">
         <v>75</v>
@@ -5100,15 +5100,15 @@
       </c>
       <c r="F63" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F63" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>ThankGod</v>
       </c>
       <c r="G63" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G63" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>ThankGod</v>
       </c>
       <c r="H63" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H63" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>MadeIt</v>
       </c>
       <c r="I63">
         <v>100</v>
@@ -5144,15 +5144,15 @@
       </c>
       <c r="F64" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F64" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>HardTimes</v>
       </c>
       <c r="G64" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G64" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>HardTimes</v>
       </c>
       <c r="H64" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H64" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="I64">
         <v>200</v>
@@ -5188,15 +5188,15 @@
       </c>
       <c r="F65" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F65" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>HELPME</v>
       </c>
       <c r="G65" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G65" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>Depressing</v>
       </c>
       <c r="H65" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H65" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>WeLostThem</v>
       </c>
       <c r="I65">
         <v>175</v>
@@ -5240,7 +5240,7 @@
       </c>
       <c r="H66" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H66" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="I66">
         <v>350</v>
@@ -5276,15 +5276,15 @@
       </c>
       <c r="F67" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F67" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="G67" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G67" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="H67" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H67" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>LONGWaitTimes</v>
       </c>
       <c r="I67">
         <v>250</v>
@@ -5324,11 +5324,11 @@
       </c>
       <c r="G68" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G68" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="H68" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H68" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="I68">
         <v>75</v>
@@ -5364,15 +5364,15 @@
       </c>
       <c r="F69" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F69" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="G69" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G69" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="H69" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H69" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>WEStrong</v>
       </c>
       <c r="I69">
         <v>50</v>
@@ -5408,15 +5408,15 @@
       </c>
       <c r="F70" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F70" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>Desperate</v>
       </c>
       <c r="G70" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G70" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="H70" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H70" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>Outcast</v>
       </c>
       <c r="I70">
         <v>150</v>
@@ -5452,15 +5452,15 @@
       </c>
       <c r="F71" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F71" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="G71" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G71" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>Outcast</v>
       </c>
       <c r="H71" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H71" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>SplitUp</v>
       </c>
       <c r="I71">
         <v>200</v>
@@ -5496,11 +5496,11 @@
       </c>
       <c r="F72" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F72" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>Messiah</v>
       </c>
       <c r="G72" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G72" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="H72" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H72" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -5544,11 +5544,11 @@
       </c>
       <c r="G73" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G73" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="H73" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H73" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>Messiah</v>
       </c>
       <c r="I73">
         <v>150</v>
@@ -5584,15 +5584,15 @@
       </c>
       <c r="F74" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F74" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>VoteAgain</v>
       </c>
       <c r="G74" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G74" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>KeepThemIN!</v>
+        <v>VoteAgain</v>
       </c>
       <c r="H74" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H74" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="I74">
         <v>75</v>
@@ -5628,15 +5628,15 @@
       </c>
       <c r="F75" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F75" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>People'sVoice</v>
+        <v>InGoodHands</v>
       </c>
       <c r="G75" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G75" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>InGoodHands</v>
       </c>
       <c r="H75" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H75" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v>VoteAgain</v>
       </c>
       <c r="I75">
         <v>50</v>
@@ -5648,7 +5648,7 @@
         <v>150</v>
       </c>
       <c r="L75" s="20" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="M75" s="19" t="s">
         <v>277</v>
@@ -5672,11 +5672,11 @@
       </c>
       <c r="F76" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F76" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>NoFaith</v>
       </c>
       <c r="G76" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G76" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="H76" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H76" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -5716,15 +5716,15 @@
       </c>
       <c r="F77" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F77" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="G77" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G77" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>WhatAJoke</v>
       </c>
       <c r="H77" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H77" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="I77">
         <v>125</v>
@@ -5760,15 +5760,15 @@
       </c>
       <c r="F78" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F78" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>RiotTIME</v>
       </c>
       <c r="G78" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G78" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="H78" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H78" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>RiotTIME</v>
       </c>
       <c r="I78">
         <v>200</v>
@@ -5804,15 +5804,15 @@
       </c>
       <c r="F79" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F79" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>RiotTIME</v>
       </c>
       <c r="G79" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G79" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>BurnItDOWN</v>
       </c>
       <c r="H79" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H79" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RiotTIME</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="I79">
         <v>125</v>
@@ -5848,15 +5848,15 @@
       </c>
       <c r="F80" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F80" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="G80" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G80" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="H80" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H80" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FightBackTeam!</v>
+        <v>Justice</v>
       </c>
       <c r="I80">
         <v>75</v>
@@ -5892,15 +5892,15 @@
       </c>
       <c r="F81" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F81" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>BeSafe</v>
       </c>
       <c r="G81" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G81" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>Justified!</v>
       </c>
       <c r="H81" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H81" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>Hero</v>
       </c>
       <c r="I81">
         <v>100</v>
@@ -5936,15 +5936,15 @@
       </c>
       <c r="F82" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F82" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>Lowlife</v>
       </c>
       <c r="G82" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G82" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>SoTragic</v>
       </c>
       <c r="H82" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H82" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>FreeThem</v>
       </c>
       <c r="I82">
         <v>225</v>
@@ -5980,7 +5980,7 @@
       </c>
       <c r="F83" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F83" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FreeThem</v>
+        <v>WhatAShame</v>
       </c>
       <c r="G83" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G83" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -5988,7 +5988,7 @@
       </c>
       <c r="H83" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H83" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>TooSoon</v>
       </c>
       <c r="I83">
         <v>175</v>
@@ -6028,11 +6028,11 @@
       </c>
       <c r="G84" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G84" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>AskingForIt</v>
       </c>
       <c r="H84" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H84" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="I84">
         <v>325</v>
@@ -6068,7 +6068,7 @@
       </c>
       <c r="F85" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F85" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="G85" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G85" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -6076,7 +6076,7 @@
       </c>
       <c r="H85" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H85" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="I85">
         <v>200</v>
@@ -6112,15 +6112,15 @@
       </c>
       <c r="F86" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F86" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="G86" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G86" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>MadeIt</v>
       </c>
       <c r="H86" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H86" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>ThankGod</v>
       </c>
       <c r="I86">
         <v>75</v>
@@ -6156,15 +6156,15 @@
       </c>
       <c r="F87" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F87" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>ThankGod</v>
       </c>
       <c r="G87" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G87" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>BackToUs</v>
       </c>
       <c r="H87" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H87" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="I87">
         <v>100</v>
@@ -6204,11 +6204,11 @@
       </c>
       <c r="G88" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G88" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>HELPME</v>
       </c>
       <c r="H88" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H88" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HELPME</v>
+        <v>God'sPlan</v>
       </c>
       <c r="I88">
         <v>200</v>
@@ -6244,15 +6244,15 @@
       </c>
       <c r="F89" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F89" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>Drained</v>
       </c>
       <c r="G89" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G89" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>Drained</v>
       </c>
       <c r="H89" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H89" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>WeLostThem</v>
       </c>
       <c r="I89">
         <v>175</v>
@@ -6288,7 +6288,7 @@
       </c>
       <c r="F90" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F90" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>CrapStaff</v>
       </c>
       <c r="G90" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G90" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -6296,7 +6296,7 @@
       </c>
       <c r="H90" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H90" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="I90">
         <v>350</v>
@@ -6332,15 +6332,15 @@
       </c>
       <c r="F91" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F91" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>CrapStaff</v>
       </c>
       <c r="G91" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G91" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="H91" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H91" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>Refund</v>
       </c>
       <c r="I91">
         <v>250</v>
@@ -6376,15 +6376,15 @@
       </c>
       <c r="F92" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F92" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WEStrong</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="G92" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G92" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="H92" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H92" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="I92">
         <v>75</v>
@@ -6420,15 +6420,15 @@
       </c>
       <c r="F93" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F93" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="G93" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G93" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>CommunityBuild</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="H93" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H93" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="I93">
         <v>50</v>
@@ -6464,7 +6464,7 @@
       </c>
       <c r="F94" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F94" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="G94" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G94" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -6472,7 +6472,7 @@
       </c>
       <c r="H94" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H94" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>Desperate</v>
       </c>
       <c r="I94">
         <v>150</v>
@@ -6508,15 +6508,15 @@
       </c>
       <c r="F95" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F95" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="G95" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G95" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="H95" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H95" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="I95">
         <v>200</v>
@@ -6556,11 +6556,11 @@
       </c>
       <c r="G96" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G96" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>OurLastHope</v>
       </c>
       <c r="H96" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H96" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>Messiah</v>
       </c>
       <c r="I96">
         <v>400</v>
@@ -6596,11 +6596,11 @@
       </c>
       <c r="F97" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F97" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>NecessaryEvil</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="G97" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G97" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="H97" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H97" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -6644,11 +6644,11 @@
       </c>
       <c r="G98" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G98" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>VoteAgain</v>
       </c>
       <c r="H98" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H98" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v xml:space="preserve">Saviours </v>
       </c>
       <c r="I98">
         <v>75</v>
@@ -6684,15 +6684,15 @@
       </c>
       <c r="F99" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F99" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v xml:space="preserve">Saviours </v>
       </c>
       <c r="G99" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G99" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>InGoodHands</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="H99" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H99" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>People'sVoice</v>
       </c>
       <c r="I99">
         <v>50</v>
@@ -6704,7 +6704,7 @@
         <v>150</v>
       </c>
       <c r="L99" s="20" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="M99" s="19" t="s">
         <v>301</v>
@@ -6728,15 +6728,15 @@
       </c>
       <c r="F100" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F100" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>ItsOver</v>
       </c>
       <c r="G100" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G100" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>NoFaith</v>
       </c>
       <c r="H100" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H100" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="I100">
         <v>100</v>
@@ -6772,15 +6772,15 @@
       </c>
       <c r="F101" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F101" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>ItsOver</v>
       </c>
       <c r="G101" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G101" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="H101" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H101" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NoFaith</v>
+        <v>I'maSitDown</v>
       </c>
       <c r="I101">
         <v>125</v>
@@ -6816,15 +6816,15 @@
       </c>
       <c r="F102" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F102" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>RaidingNight</v>
       </c>
       <c r="G102" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G102" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="H102" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H102" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="I102">
         <v>200</v>
@@ -6860,15 +6860,15 @@
       </c>
       <c r="F103" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F103" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>BurnItDOWN</v>
       </c>
       <c r="G103" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G103" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="H103" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H103" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>BurnItDOWN</v>
       </c>
       <c r="I103">
         <v>125</v>
@@ -6904,15 +6904,15 @@
       </c>
       <c r="F104" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F104" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>StrongerTogether</v>
       </c>
       <c r="G104" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G104" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="H104" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H104" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="I104">
         <v>75</v>
@@ -6952,11 +6952,11 @@
       </c>
       <c r="G105" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G105" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>Justice</v>
       </c>
       <c r="H105" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H105" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>Justified!</v>
       </c>
       <c r="I105">
         <v>100</v>
@@ -6992,15 +6992,15 @@
       </c>
       <c r="F106" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F106" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>PrayForThem</v>
       </c>
       <c r="G106" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G106" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FreeThem</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="H106" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H106" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>WhatAShame</v>
       </c>
       <c r="I106">
         <v>225</v>
@@ -7036,7 +7036,7 @@
       </c>
       <c r="F107" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F107" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>Lowlife</v>
       </c>
       <c r="G107" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G107" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -7080,7 +7080,7 @@
       </c>
       <c r="F108" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F108" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>PaybackTime</v>
       </c>
       <c r="G108" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G108" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -7088,7 +7088,7 @@
       </c>
       <c r="H108" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H108" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="I108">
         <v>325</v>
@@ -7124,15 +7124,15 @@
       </c>
       <c r="F109" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F109" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>AskingForIt</v>
       </c>
       <c r="G109" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G109" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="H109" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H109" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>AskingForIt</v>
       </c>
       <c r="I109">
         <v>200</v>
@@ -7168,15 +7168,15 @@
       </c>
       <c r="F110" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F110" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>BestWishes</v>
       </c>
       <c r="G110" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G110" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>MadeIt</v>
       </c>
       <c r="H110" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H110" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>100Sober</v>
       </c>
       <c r="I110">
         <v>75</v>
@@ -7212,15 +7212,15 @@
       </c>
       <c r="F111" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F111" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>100Sober</v>
+        <v>BestWishes</v>
       </c>
       <c r="G111" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G111" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Hugs&amp;Kisses</v>
+        <v>MadeIt</v>
       </c>
       <c r="H111" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H111" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>ThankGod</v>
       </c>
       <c r="I111">
         <v>100</v>
@@ -7256,15 +7256,15 @@
       </c>
       <c r="F112" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F112" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>I'mSoLost</v>
       </c>
       <c r="G112" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G112" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>Depressing</v>
       </c>
       <c r="H112" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H112" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="I112">
         <v>200</v>
@@ -7300,15 +7300,15 @@
       </c>
       <c r="F113" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F113" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>HELPME</v>
       </c>
       <c r="G113" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G113" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>HardTimes</v>
       </c>
       <c r="H113" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H113" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>Drained</v>
       </c>
       <c r="I113">
         <v>175</v>
@@ -7344,15 +7344,15 @@
       </c>
       <c r="F114" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F114" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="G114" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G114" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>LONGWaitTimes</v>
       </c>
       <c r="H114" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H114" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="I114">
         <v>350</v>
@@ -7388,15 +7388,15 @@
       </c>
       <c r="F115" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F115" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>CrapStaff</v>
       </c>
       <c r="G115" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G115" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="H115" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H115" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="I115">
         <v>250</v>
@@ -7436,11 +7436,11 @@
       </c>
       <c r="G116" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G116" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>CommunityBuild</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="H116" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H116" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="I116">
         <v>75</v>
@@ -7476,15 +7476,15 @@
       </c>
       <c r="F117" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F117" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>WEStrong</v>
       </c>
       <c r="G117" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G117" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="H117" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H117" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="I117">
         <v>50</v>
@@ -7520,15 +7520,15 @@
       </c>
       <c r="F118" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F118" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="G118" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G118" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="H118" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H118" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>Desperate</v>
       </c>
       <c r="I118">
         <v>150</v>
@@ -7564,15 +7564,15 @@
       </c>
       <c r="F119" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F119" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="G119" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G119" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>Outcast</v>
       </c>
       <c r="H119" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H119" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>Outcast</v>
       </c>
       <c r="I119">
         <v>200</v>
@@ -7608,15 +7608,15 @@
       </c>
       <c r="F120" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F120" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="G120" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G120" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>NecessaryEvil</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="H120" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H120" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>OurLastHope</v>
       </c>
       <c r="I120">
         <v>400</v>
@@ -7652,15 +7652,15 @@
       </c>
       <c r="F121" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F121" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="G121" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G121" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="H121" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H121" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="I121">
         <v>150</v>
@@ -7696,15 +7696,15 @@
       </c>
       <c r="F122" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F122" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v>RepeatElection</v>
       </c>
       <c r="G122" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G122" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>VoteAgain</v>
       </c>
       <c r="H122" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H122" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="I122">
         <v>75</v>
@@ -7716,7 +7716,7 @@
         <v>100</v>
       </c>
       <c r="L122" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="M122" s="19" t="s">
         <v>324</v>
@@ -7740,15 +7740,15 @@
       </c>
       <c r="F123" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F123" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>People'sVoice</v>
       </c>
       <c r="G123" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G123" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>ReElect!!!</v>
       </c>
       <c r="H123" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H123" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="I123">
         <v>50</v>
@@ -7784,15 +7784,15 @@
       </c>
       <c r="F124" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F124" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="G124" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G124" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="H124" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H124" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="I124">
         <v>100</v>
@@ -7828,7 +7828,7 @@
       </c>
       <c r="F125" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F125" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="G125" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G125" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -7836,7 +7836,7 @@
       </c>
       <c r="H125" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H125" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="I125">
         <v>125</v>
@@ -7872,15 +7872,15 @@
       </c>
       <c r="F126" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F126" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>CoupDeTahhh</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="G126" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G126" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>RiotTIME</v>
       </c>
       <c r="H126" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H126" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>ToTheTorches!</v>
       </c>
       <c r="I126">
         <v>200</v>
@@ -7916,7 +7916,7 @@
       </c>
       <c r="F127" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F127" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="G127" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G127" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -7924,7 +7924,7 @@
       </c>
       <c r="H127" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H127" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="I127">
         <v>125</v>
@@ -7960,15 +7960,15 @@
       </c>
       <c r="F128" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F128" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>Justified!</v>
       </c>
       <c r="G128" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G128" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>Justice</v>
       </c>
       <c r="H128" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H128" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="I128">
         <v>75</v>
@@ -8004,15 +8004,15 @@
       </c>
       <c r="F129" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F129" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>BeSafe</v>
       </c>
       <c r="G129" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G129" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>Justified!</v>
       </c>
       <c r="H129" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H129" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>BeSafe</v>
       </c>
       <c r="I129">
         <v>100</v>
@@ -8048,15 +8048,15 @@
       </c>
       <c r="F130" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F130" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>FreeThem</v>
       </c>
       <c r="G130" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G130" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FreeThem</v>
+        <v>PrayForThem</v>
       </c>
       <c r="H130" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H130" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>Lowlife</v>
       </c>
       <c r="I130">
         <v>225</v>
@@ -8092,11 +8092,11 @@
       </c>
       <c r="F131" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F131" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="G131" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G131" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="H131" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H131" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -8136,15 +8136,15 @@
       </c>
       <c r="F132" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F132" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="G132" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G132" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="H132" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H132" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="I132">
         <v>325</v>
@@ -8180,15 +8180,15 @@
       </c>
       <c r="F133" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F133" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="G133" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G133" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>Despicable!</v>
       </c>
       <c r="H133" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H133" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="I133">
         <v>200</v>
@@ -8224,15 +8224,15 @@
       </c>
       <c r="F134" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F134" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="G134" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G134" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>100Sober</v>
       </c>
       <c r="H134" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H134" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>MadeIt</v>
       </c>
       <c r="I134">
         <v>75</v>
@@ -8268,15 +8268,15 @@
       </c>
       <c r="F135" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F135" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="G135" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G135" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>100Sober</v>
+        <v>ThankGod</v>
       </c>
       <c r="H135" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H135" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>Recovered:)</v>
       </c>
       <c r="I135">
         <v>100</v>
@@ -8316,7 +8316,7 @@
       </c>
       <c r="G136" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G136" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>Drained</v>
       </c>
       <c r="H136" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H136" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -8356,7 +8356,7 @@
       </c>
       <c r="F137" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F137" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>God'sPlan</v>
       </c>
       <c r="G137" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G137" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -8364,7 +8364,7 @@
       </c>
       <c r="H137" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H137" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>HELPME</v>
       </c>
       <c r="I137">
         <v>175</v>
@@ -8400,15 +8400,15 @@
       </c>
       <c r="F138" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F138" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>Refund</v>
       </c>
       <c r="G138" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G138" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="H138" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H138" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="I138">
         <v>350</v>
@@ -8444,15 +8444,15 @@
       </c>
       <c r="F139" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F139" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="G139" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G139" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="H139" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H139" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>LONGWaitTimes</v>
       </c>
       <c r="I139">
         <v>250</v>
@@ -8488,15 +8488,15 @@
       </c>
       <c r="F140" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F140" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>CommunityBuild</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="G140" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G140" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>CommunityBuild</v>
+        <v>WEStrong</v>
       </c>
       <c r="H140" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H140" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="I140">
         <v>75</v>
@@ -8536,11 +8536,11 @@
       </c>
       <c r="G141" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G141" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="H141" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H141" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="I141">
         <v>50</v>
@@ -8576,15 +8576,15 @@
       </c>
       <c r="F142" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F142" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="G142" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G142" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>Desperate</v>
       </c>
       <c r="H142" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H142" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="I142">
         <v>150</v>
@@ -8620,7 +8620,7 @@
       </c>
       <c r="F143" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F143" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="G143" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G143" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -8628,7 +8628,7 @@
       </c>
       <c r="H143" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H143" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="I143">
         <v>200</v>
@@ -8664,15 +8664,15 @@
       </c>
       <c r="F144" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F144" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="G144" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G144" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="H144" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H144" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>OurLastHope</v>
       </c>
       <c r="I144">
         <v>400</v>
@@ -8684,7 +8684,7 @@
         <v>100</v>
       </c>
       <c r="L144" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="M144" t="s">
         <v>346</v>
@@ -8712,11 +8712,11 @@
       </c>
       <c r="G145" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G145" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="H145" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H145" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="I145">
         <v>150</v>
@@ -8752,15 +8752,15 @@
       </c>
       <c r="F146" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F146" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>People'sVoice</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="G146" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G146" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="H146" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H146" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v>InGoodHands</v>
       </c>
       <c r="I146">
         <v>75</v>
@@ -8772,7 +8772,7 @@
         <v>100</v>
       </c>
       <c r="L146" s="20" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="M146" s="19" t="s">
         <v>348</v>
@@ -8796,15 +8796,15 @@
       </c>
       <c r="F147" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F147" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>InGoodHands</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="G147" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G147" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>InGoodHands</v>
       </c>
       <c r="H147" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H147" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v xml:space="preserve">Saviours </v>
       </c>
       <c r="I147">
         <v>50</v>
@@ -8816,7 +8816,7 @@
         <v>150</v>
       </c>
       <c r="L147" s="8" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="M147" t="s">
         <v>349</v>
@@ -8840,11 +8840,11 @@
       </c>
       <c r="F148" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F148" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>I'maSitDown</v>
       </c>
       <c r="G148" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G148" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NoFaith</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="H148" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H148" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -8884,15 +8884,15 @@
       </c>
       <c r="F149" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F149" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="G149" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G149" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NoFaith</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="H149" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H149" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NoFaith</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="I149">
         <v>125</v>
@@ -8928,15 +8928,15 @@
       </c>
       <c r="F150" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F150" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="G150" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G150" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="H150" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H150" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>RaidingNight</v>
       </c>
       <c r="I150">
         <v>200</v>
@@ -8976,11 +8976,11 @@
       </c>
       <c r="G151" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G151" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>RaidingNight</v>
       </c>
       <c r="H151" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H151" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>RaidingNight</v>
       </c>
       <c r="I151">
         <v>125</v>
@@ -9016,15 +9016,15 @@
       </c>
       <c r="F152" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F152" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FightBackTeam!</v>
+        <v>ComeTogether!!</v>
       </c>
       <c r="G152" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G152" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="H152" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H152" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="I152">
         <v>75</v>
@@ -9060,15 +9060,15 @@
       </c>
       <c r="F153" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F153" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="G153" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G153" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>Hero</v>
       </c>
       <c r="H153" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H153" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>BeSafe</v>
       </c>
       <c r="I153">
         <v>100</v>
@@ -9104,15 +9104,15 @@
       </c>
       <c r="F154" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F154" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>Pathetic</v>
       </c>
       <c r="G154" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G154" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>WhatAShame</v>
       </c>
       <c r="H154" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H154" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>FreeThem</v>
       </c>
       <c r="I154">
         <v>225</v>
@@ -9148,15 +9148,15 @@
       </c>
       <c r="F155" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F155" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FreeThem</v>
+        <v>SoTragic</v>
       </c>
       <c r="G155" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G155" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>WhatAShame</v>
       </c>
       <c r="H155" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H155" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>Lowlife</v>
       </c>
       <c r="I155">
         <v>175</v>
@@ -9196,11 +9196,11 @@
       </c>
       <c r="G156" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G156" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>Despicable!</v>
       </c>
       <c r="H156" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H156" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="I156">
         <v>325</v>
@@ -9236,15 +9236,15 @@
       </c>
       <c r="F157" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F157" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>DeathCollection</v>
       </c>
       <c r="G157" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G157" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>Despicable!</v>
       </c>
       <c r="H157" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H157" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="I157">
         <v>200</v>
@@ -9284,11 +9284,11 @@
       </c>
       <c r="G158" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G158" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Hugs&amp;Kisses</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="H158" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H158" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Hugs&amp;Kisses</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="I158">
         <v>75</v>
@@ -9324,15 +9324,15 @@
       </c>
       <c r="F159" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F159" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>ThankGod</v>
       </c>
       <c r="G159" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G159" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>100Sober</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="H159" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H159" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>100Sober</v>
       </c>
       <c r="I159">
         <v>100</v>
@@ -9368,15 +9368,15 @@
       </c>
       <c r="F160" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F160" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>I'mSoLost</v>
       </c>
       <c r="G160" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G160" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Depressing</v>
+        <v>God'sPlan</v>
       </c>
       <c r="H160" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H160" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Depressing</v>
+        <v>God'sPlan</v>
       </c>
       <c r="I160">
         <v>200</v>
@@ -9412,15 +9412,15 @@
       </c>
       <c r="F161" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F161" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HELPME</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="G161" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G161" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>Drained</v>
       </c>
       <c r="H161" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H161" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>Drained</v>
       </c>
       <c r="I161">
         <v>175</v>
@@ -9456,15 +9456,15 @@
       </c>
       <c r="F162" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F162" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>CrapStaff</v>
       </c>
       <c r="G162" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G162" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>Refund</v>
       </c>
       <c r="H162" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H162" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>CrapStaff</v>
       </c>
       <c r="I162">
         <v>350</v>
@@ -9500,11 +9500,11 @@
       </c>
       <c r="F163" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F163" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="G163" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G163" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="H163" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H163" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -9544,15 +9544,15 @@
       </c>
       <c r="F164" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F164" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="G164" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G164" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="H164" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H164" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WEStrong</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="I164">
         <v>75</v>
@@ -9588,7 +9588,7 @@
       </c>
       <c r="F165" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F165" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="G165" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G165" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -9596,7 +9596,7 @@
       </c>
       <c r="H165" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H165" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>CommunityBuild</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="I165">
         <v>50</v>
@@ -9636,11 +9636,11 @@
       </c>
       <c r="G166" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G166" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="H166" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H166" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WeNeedChange</v>
+        <v>SplitUp</v>
       </c>
       <c r="I166">
         <v>150</v>
@@ -9676,7 +9676,7 @@
       </c>
       <c r="F167" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F167" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="G167" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G167" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -9720,15 +9720,15 @@
       </c>
       <c r="F168" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F168" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="G168" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G168" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>Messiah</v>
       </c>
       <c r="H168" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H168" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="I168">
         <v>400</v>
@@ -9764,7 +9764,7 @@
       </c>
       <c r="F169" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F169" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="G169" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G169" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -9772,7 +9772,7 @@
       </c>
       <c r="H169" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H169" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>NecessaryEvil</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="I169">
         <v>150</v>
@@ -9812,11 +9812,11 @@
       </c>
       <c r="G170" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G170" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v>RepeatElection</v>
       </c>
       <c r="H170" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H170" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v xml:space="preserve">Saviours </v>
       </c>
       <c r="I170">
         <v>75</v>
@@ -9828,7 +9828,7 @@
         <v>100</v>
       </c>
       <c r="L170" s="7" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="M170" t="s">
         <v>372</v>
@@ -9852,15 +9852,15 @@
       </c>
       <c r="F171" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F171" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="G171" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G171" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v>ReElect!!!</v>
       </c>
       <c r="H171" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H171" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>People'sVoice</v>
       </c>
       <c r="I171">
         <v>50</v>
@@ -9872,7 +9872,7 @@
         <v>150</v>
       </c>
       <c r="L171" s="20" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="M171" s="19" t="s">
         <v>373</v>
@@ -9896,15 +9896,15 @@
       </c>
       <c r="F172" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F172" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>I'maSitDown</v>
       </c>
       <c r="G172" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G172" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="H172" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H172" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>NoFaith</v>
       </c>
       <c r="I172">
         <v>100</v>
@@ -9944,11 +9944,11 @@
       </c>
       <c r="G173" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G173" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="H173" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H173" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>I'maSitDown</v>
       </c>
       <c r="I173">
         <v>125</v>
@@ -9988,11 +9988,11 @@
       </c>
       <c r="G174" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G174" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>CoupDeTahhh</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="H174" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H174" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>RiotTIME</v>
       </c>
       <c r="I174">
         <v>200</v>
@@ -10028,15 +10028,15 @@
       </c>
       <c r="F175" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F175" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>RaidingNight</v>
       </c>
       <c r="G175" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G175" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>RiotTIME</v>
       </c>
       <c r="H175" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H175" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>CoupDeTahhh</v>
+        <v>BurnItDOWN</v>
       </c>
       <c r="I175">
         <v>125</v>
@@ -10072,15 +10072,15 @@
       </c>
       <c r="F176" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F176" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="G176" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G176" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>ComeTogether!!</v>
       </c>
       <c r="H176" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H176" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>Justified!</v>
       </c>
       <c r="I176">
         <v>75</v>
@@ -10116,15 +10116,15 @@
       </c>
       <c r="F177" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F177" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FightBackTeam!</v>
+        <v>Hero</v>
       </c>
       <c r="G177" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G177" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>StrongerTogether</v>
       </c>
       <c r="H177" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H177" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FightBackTeam!</v>
+        <v>Hero</v>
       </c>
       <c r="I177">
         <v>100</v>
@@ -10160,15 +10160,15 @@
       </c>
       <c r="F178" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F178" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>FreeThem</v>
       </c>
       <c r="G178" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G178" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>FreeThem</v>
       </c>
       <c r="H178" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H178" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>FreeThem</v>
       </c>
       <c r="I178">
         <v>225</v>
@@ -10204,15 +10204,15 @@
       </c>
       <c r="F179" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F179" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>Lowlife</v>
       </c>
       <c r="G179" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G179" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>WhatAShame</v>
       </c>
       <c r="H179" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H179" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>WhatAShame</v>
       </c>
       <c r="I179">
         <v>175</v>
@@ -10248,15 +10248,15 @@
       </c>
       <c r="F180" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F180" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="G180" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G180" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>AskingForIt</v>
       </c>
       <c r="H180" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H180" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="I180">
         <v>325</v>
@@ -10292,11 +10292,11 @@
       </c>
       <c r="F181" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F181" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="G181" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G181" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="H181" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H181" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -10336,11 +10336,11 @@
       </c>
       <c r="F182" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F182" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>MadeIt</v>
       </c>
       <c r="G182" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G182" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>ThankGod</v>
       </c>
       <c r="H182" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H182" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -10380,15 +10380,15 @@
       </c>
       <c r="F183" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F183" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>ThankGod</v>
       </c>
       <c r="G183" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G183" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>100Sober</v>
+        <v>BackToUs</v>
       </c>
       <c r="H183" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H183" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>MadeIt</v>
       </c>
       <c r="I183">
         <v>100</v>
@@ -10424,7 +10424,7 @@
       </c>
       <c r="F184" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F184" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>HardTimes</v>
       </c>
       <c r="G184" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G184" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -10432,7 +10432,7 @@
       </c>
       <c r="H184" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H184" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Depressing</v>
+        <v>HELPME</v>
       </c>
       <c r="I184">
         <v>200</v>
@@ -10472,11 +10472,11 @@
       </c>
       <c r="G185" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G185" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>Depressing</v>
       </c>
       <c r="H185" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H185" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>God'sPlan</v>
       </c>
       <c r="I185">
         <v>175</v>
@@ -10512,15 +10512,15 @@
       </c>
       <c r="F186" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F186" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="G186" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G186" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="H186" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H186" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="I186">
         <v>350</v>
@@ -10556,15 +10556,15 @@
       </c>
       <c r="F187" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F187" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="G187" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G187" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="H187" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H187" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="I187">
         <v>250</v>
@@ -10604,11 +10604,11 @@
       </c>
       <c r="G188" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G188" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>WEStrong</v>
       </c>
       <c r="H188" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H188" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WEStrong</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="I188">
         <v>75</v>
@@ -10644,15 +10644,15 @@
       </c>
       <c r="F189" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F189" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>ALWAYSSupport</v>
       </c>
       <c r="G189" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G189" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="H189" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H189" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="I189">
         <v>50</v>
@@ -10692,11 +10692,11 @@
       </c>
       <c r="G190" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G190" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="H190" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H190" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="I190">
         <v>150</v>
@@ -10736,11 +10736,11 @@
       </c>
       <c r="G191" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G191" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>Outcast</v>
       </c>
       <c r="H191" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H191" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>Desperate</v>
       </c>
       <c r="I191">
         <v>200</v>
@@ -10776,15 +10776,15 @@
       </c>
       <c r="F192" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F192" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="G192" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G192" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>Messiah</v>
       </c>
       <c r="H192" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H192" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>Messiah</v>
       </c>
       <c r="I192">
         <v>400</v>
@@ -10820,15 +10820,15 @@
       </c>
       <c r="F193" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F193" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="G193" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G193" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="H193" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H193" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>OurLastHope</v>
       </c>
       <c r="I193">
         <v>150</v>
@@ -10864,15 +10864,15 @@
       </c>
       <c r="F194" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F194" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="G194" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G194" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="H194" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H194" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>People'sVoice</v>
       </c>
       <c r="I194">
         <v>75</v>
@@ -10908,7 +10908,7 @@
       </c>
       <c r="F195" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F195" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>People'sVoice</v>
       </c>
       <c r="G195" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G195" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -10916,7 +10916,7 @@
       </c>
       <c r="H195" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H195" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>People'sVoice</v>
+        <v>RepeatElection</v>
       </c>
       <c r="I195">
         <v>50</v>
@@ -10928,7 +10928,7 @@
         <v>150</v>
       </c>
       <c r="L195" s="7" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="M195" t="s">
         <v>397</v>
@@ -10952,15 +10952,15 @@
       </c>
       <c r="F196" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F196" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="G196" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G196" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>WhatAJoke</v>
       </c>
       <c r="H196" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H196" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="I196">
         <v>100</v>
@@ -10996,11 +10996,11 @@
       </c>
       <c r="F197" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F197" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="G197" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G197" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>ItsOver</v>
       </c>
       <c r="H197" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H197" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -11040,15 +11040,15 @@
       </c>
       <c r="F198" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F198" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>RaidingNight</v>
       </c>
       <c r="G198" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G198" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="H198" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H198" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="I198">
         <v>200</v>
@@ -11088,7 +11088,7 @@
       </c>
       <c r="G199" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G199" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="H199" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H199" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -11128,15 +11128,15 @@
       </c>
       <c r="F200" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F200" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>Justice</v>
       </c>
       <c r="G200" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G200" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="H200" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H200" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="I200">
         <v>75</v>
@@ -11172,15 +11172,15 @@
       </c>
       <c r="F201" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F201" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>BeSafe</v>
       </c>
       <c r="G201" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G201" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="H201" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H201" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>ComeTogether!!</v>
       </c>
       <c r="I201">
         <v>100</v>
@@ -11216,15 +11216,15 @@
       </c>
       <c r="F202" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F202" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>TooSoon</v>
       </c>
       <c r="G202" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G202" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>Pathetic</v>
       </c>
       <c r="H202" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H202" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>WhatAShame</v>
       </c>
       <c r="I202">
         <v>225</v>
@@ -11260,7 +11260,7 @@
       </c>
       <c r="F203" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F203" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FreeThem</v>
+        <v>TooSoon</v>
       </c>
       <c r="G203" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G203" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -11268,7 +11268,7 @@
       </c>
       <c r="H203" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H203" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>Pathetic</v>
       </c>
       <c r="I203">
         <v>175</v>
@@ -11304,15 +11304,15 @@
       </c>
       <c r="F204" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F204" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>DeathCollection</v>
       </c>
       <c r="G204" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G204" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="H204" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H204" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>AskingForIt</v>
       </c>
       <c r="I204">
         <v>325</v>
@@ -11348,15 +11348,15 @@
       </c>
       <c r="F205" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F205" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="G205" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G205" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="H205" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H205" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>DeathCollection</v>
       </c>
       <c r="I205">
         <v>200</v>
@@ -11392,7 +11392,7 @@
       </c>
       <c r="F206" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F206" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>Recovered:)</v>
       </c>
       <c r="G206" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G206" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -11400,7 +11400,7 @@
       </c>
       <c r="H206" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H206" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>100Sober</v>
       </c>
       <c r="I206">
         <v>75</v>
@@ -11436,15 +11436,15 @@
       </c>
       <c r="F207" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F207" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>MadeIt</v>
       </c>
       <c r="G207" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G207" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>Recovered:)</v>
       </c>
       <c r="H207" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H207" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>Recovered:)</v>
       </c>
       <c r="I207">
         <v>100</v>
@@ -11480,15 +11480,15 @@
       </c>
       <c r="F208" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F208" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>God'sPlan</v>
       </c>
       <c r="G208" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G208" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HELPME</v>
+        <v>Depressing</v>
       </c>
       <c r="H208" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H208" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>Drained</v>
       </c>
       <c r="I208">
         <v>200</v>
@@ -11524,15 +11524,15 @@
       </c>
       <c r="F209" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F209" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Depressing</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="G209" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G209" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>HELPME</v>
       </c>
       <c r="H209" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H209" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>I'mSoLost</v>
       </c>
       <c r="I209">
         <v>175</v>
@@ -11572,11 +11572,11 @@
       </c>
       <c r="G210" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G210" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="H210" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H210" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="I210">
         <v>350</v>
@@ -11612,7 +11612,7 @@
       </c>
       <c r="F211" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F211" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="G211" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G211" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -11620,7 +11620,7 @@
       </c>
       <c r="H211" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H211" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="I211">
         <v>250</v>
@@ -11660,11 +11660,11 @@
       </c>
       <c r="G212" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G212" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WEStrong</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="H212" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H212" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>ALWAYSSupport</v>
       </c>
       <c r="I212">
         <v>75</v>
@@ -11700,15 +11700,15 @@
       </c>
       <c r="F213" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F213" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>WEStrong</v>
       </c>
       <c r="G213" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G213" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="H213" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H213" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WEStrong</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="I213">
         <v>50</v>
@@ -11744,7 +11744,7 @@
       </c>
       <c r="F214" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F214" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="G214" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G214" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -11752,7 +11752,7 @@
       </c>
       <c r="H214" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H214" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>Outcast</v>
       </c>
       <c r="I214">
         <v>150</v>
@@ -11788,15 +11788,15 @@
       </c>
       <c r="F215" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F215" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="G215" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G215" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WeNeedChange</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="H215" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H215" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="I215">
         <v>200</v>
@@ -11832,15 +11832,15 @@
       </c>
       <c r="F216" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F216" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="G216" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G216" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="H216" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H216" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="I216">
         <v>400</v>
@@ -11876,15 +11876,15 @@
       </c>
       <c r="F217" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F217" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="G217" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G217" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>NecessaryEvil</v>
+        <v>Messiah</v>
       </c>
       <c r="H217" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H217" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="I217">
         <v>150</v>
@@ -11942,7 +11942,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>18</v>
@@ -11962,7 +11962,7 @@
         <v>71</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>74</v>
@@ -11973,13 +11973,13 @@
         <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>498</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -11987,13 +11987,13 @@
         <v>15</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C4" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>500</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -12004,10 +12004,10 @@
         <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -12015,13 +12015,13 @@
         <v>15</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C6" s="15" t="s">
+        <v>501</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>502</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -12032,10 +12032,10 @@
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -12043,7 +12043,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>72</v>
@@ -12057,7 +12057,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>73</v>
@@ -12074,10 +12074,10 @@
         <v>78</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -12085,13 +12085,13 @@
         <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -12099,13 +12099,13 @@
         <v>16</v>
       </c>
       <c r="B12" s="15" t="s">
+        <v>508</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>492</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>509</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>493</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -12119,7 +12119,7 @@
         <v>80</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -12127,13 +12127,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>511</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>493</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>512</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>494</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -12141,13 +12141,13 @@
         <v>16</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>81</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -12158,10 +12158,10 @@
         <v>77</v>
       </c>
       <c r="C16" s="15" t="s">
+        <v>514</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>515</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -12169,13 +12169,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>518</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -12183,13 +12183,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -12197,10 +12197,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>522</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>523</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>25</v>
@@ -12211,13 +12211,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>86</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -12228,10 +12228,10 @@
         <v>82</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>526</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -12242,10 +12242,10 @@
         <v>83</v>
       </c>
       <c r="C22" s="15" t="s">
+        <v>527</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>528</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -12253,13 +12253,13 @@
         <v>17</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>531</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -12267,10 +12267,10 @@
         <v>17</v>
       </c>
       <c r="B24" s="15" t="s">
+        <v>532</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>533</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>534</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>87</v>
@@ -12284,10 +12284,10 @@
         <v>84</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>535</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -12295,7 +12295,7 @@
         <v>31</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>90</v>
@@ -12309,10 +12309,10 @@
         <v>31</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>538</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>539</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>94</v>
@@ -12329,7 +12329,7 @@
         <v>91</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -12337,13 +12337,13 @@
         <v>31</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>542</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -12354,7 +12354,7 @@
         <v>89</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>95</v>
@@ -12365,13 +12365,13 @@
         <v>31</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>546</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -12379,13 +12379,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>92</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -12538,7 +12538,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -14038,7 +14038,7 @@
         <v>430</v>
       </c>
       <c r="E1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -14086,7 +14086,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E4" t="s">
         <v>427</v>
@@ -14120,7 +14120,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E6" t="s">
         <v>427</v>
@@ -14137,7 +14137,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E7" t="s">
         <v>427</v>
@@ -14154,7 +14154,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E8" t="s">
         <v>427</v>
@@ -14171,7 +14171,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E9" t="s">
         <v>427</v>
@@ -14188,7 +14188,7 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E10" t="s">
         <v>427</v>
@@ -14256,7 +14256,7 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E14" t="s">
         <v>427</v>
@@ -14273,7 +14273,7 @@
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E15" t="s">
         <v>427</v>
@@ -14290,7 +14290,7 @@
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E16" t="s">
         <v>427</v>
@@ -14307,7 +14307,7 @@
         <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E17" t="s">
         <v>427</v>
@@ -14324,7 +14324,7 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E18" t="s">
         <v>427</v>
@@ -14378,7 +14378,7 @@
         <v>449</v>
       </c>
       <c r="E21" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -14392,10 +14392,10 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E22" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -14409,7 +14409,7 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E23" t="s">
         <v>427</v>
@@ -14426,7 +14426,7 @@
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E24" t="s">
         <v>427</v>
@@ -14443,10 +14443,10 @@
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E25" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -14460,7 +14460,7 @@
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E26" t="s">
         <v>427</v>
@@ -14528,7 +14528,7 @@
         <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E30" t="s">
         <v>452</v>
@@ -14545,7 +14545,7 @@
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E31" t="s">
         <v>427</v>
@@ -14562,7 +14562,7 @@
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E32" t="s">
         <v>452</v>
@@ -14579,7 +14579,7 @@
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E33" t="s">
         <v>427</v>
@@ -14596,7 +14596,7 @@
         <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E34" t="s">
         <v>427</v>
@@ -14613,10 +14613,10 @@
         <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E35" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -14630,10 +14630,10 @@
         <v>15</v>
       </c>
       <c r="D36" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E36" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -14647,10 +14647,10 @@
         <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E37" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
   </sheetData>
@@ -14665,8 +14665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53B4979-BA2F-42C6-BF9E-77AF10AFAE50}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14716,7 +14716,7 @@
         <v>441</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -14772,7 +14772,7 @@
         <v>441</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -14786,7 +14786,7 @@
         <v>441</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -14800,7 +14800,7 @@
         <v>441</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -14842,7 +14842,7 @@
         <v>439</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>459</v>
+        <v>574</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -14856,7 +14856,7 @@
         <v>439</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -14870,7 +14870,7 @@
         <v>441</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -14884,7 +14884,7 @@
         <v>444</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -14898,7 +14898,7 @@
         <v>442</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -14912,7 +14912,7 @@
         <v>442</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -14926,7 +14926,7 @@
         <v>443</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -14940,7 +14940,7 @@
         <v>442</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -14954,7 +14954,7 @@
         <v>444</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -14968,7 +14968,7 @@
         <v>443</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -14982,7 +14982,7 @@
         <v>443</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -14996,7 +14996,7 @@
         <v>443</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -15010,7 +15010,7 @@
         <v>441</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -15024,7 +15024,7 @@
         <v>441</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -15038,7 +15038,7 @@
         <v>441</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Speech Event to Day 4 Government
</commit_message>
<xml_diff>
--- a/Source/Narrative/Game Data.xlsx
+++ b/Source/Narrative/Game Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grayn\OneDrive\Documents\short\Under Choices\UnderChoices\Source\Narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48867C21-F048-42FB-B3C1-FD3084C1C085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420641A6-5D72-4C65-9216-511F9043D53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23520" yWindow="1935" windowWidth="21165" windowHeight="12855" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Media Posts" sheetId="1" r:id="rId1"/>
@@ -2519,15 +2519,15 @@
       </c>
       <c r="F2" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F2" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>InGoodHands</v>
       </c>
       <c r="G2" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G2" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>People'sVoice</v>
+        <v>RepeatElection</v>
       </c>
       <c r="H2" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H2" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="I2">
         <v>75</v>
@@ -2563,15 +2563,15 @@
       </c>
       <c r="F3" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F3" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>People'sVoice</v>
+        <v>InGoodHands</v>
       </c>
       <c r="G3" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G3" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="H3" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H3" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>KeepThemIN!</v>
+        <v>RepeatElection</v>
       </c>
       <c r="I3">
         <v>50</v>
@@ -2607,15 +2607,15 @@
       </c>
       <c r="F4" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F4" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>I'maSitDown</v>
       </c>
       <c r="G4" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G4" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>I'maSitDown</v>
       </c>
       <c r="H4" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H4" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>WhatAJoke</v>
       </c>
       <c r="I4">
         <v>100</v>
@@ -2651,15 +2651,15 @@
       </c>
       <c r="F5" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F5" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NoFaith</v>
+        <v>ItsOver</v>
       </c>
       <c r="G5" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G5" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>NoFaith</v>
       </c>
       <c r="H5" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H5" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>I'maSitDown</v>
       </c>
       <c r="I5">
         <v>125</v>
@@ -2695,15 +2695,15 @@
       </c>
       <c r="F6" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F6" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>RiotTIME</v>
       </c>
       <c r="G6" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RiotTIME</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="H6" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H6" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="I6">
         <v>200</v>
@@ -2739,15 +2739,15 @@
       </c>
       <c r="F7" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F7" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RiotTIME</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="G7" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G7" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>RiotTIME</v>
       </c>
       <c r="H7" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="I7">
         <v>125</v>
@@ -2787,11 +2787,11 @@
       </c>
       <c r="G8" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G8" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FightBackTeam!</v>
+        <v>Justice</v>
       </c>
       <c r="H8" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H8" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>Justice</v>
       </c>
       <c r="I8">
         <v>75</v>
@@ -2827,15 +2827,15 @@
       </c>
       <c r="F9" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F9" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>Justice</v>
       </c>
       <c r="G9" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G9" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>StrongerTogether</v>
       </c>
       <c r="H9" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H9" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>Justice</v>
       </c>
       <c r="I9">
         <v>100</v>
@@ -2871,15 +2871,15 @@
       </c>
       <c r="F10" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>WhatAShame</v>
       </c>
       <c r="G10" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G10" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>TooSoon</v>
       </c>
       <c r="H10" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H10" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>TooSoon</v>
       </c>
       <c r="I10">
         <v>225</v>
@@ -2915,7 +2915,7 @@
       </c>
       <c r="F11" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>Pathetic</v>
       </c>
       <c r="G11" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G11" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -2923,7 +2923,7 @@
       </c>
       <c r="H11" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H11" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>SoTragic</v>
       </c>
       <c r="I11">
         <v>175</v>
@@ -2959,11 +2959,11 @@
       </c>
       <c r="F12" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="G12" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G12" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>AskingForIt</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>572</v>
@@ -3002,15 +3002,15 @@
       </c>
       <c r="F13" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>DeathCollection</v>
       </c>
       <c r="G13" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G13" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>PaybackTime</v>
       </c>
       <c r="H13" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H13" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>AskingForIt</v>
       </c>
       <c r="I13">
         <v>200</v>
@@ -3046,15 +3046,15 @@
       </c>
       <c r="F14" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="G14" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G14" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>Recovered:)</v>
       </c>
       <c r="H14" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H14" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Hugs&amp;Kisses</v>
+        <v>BackToUs</v>
       </c>
       <c r="I14">
         <v>75</v>
@@ -3090,15 +3090,15 @@
       </c>
       <c r="F15" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F15" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>BackToUs</v>
       </c>
       <c r="G15" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G15" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="H15" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H15" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>BackToUs</v>
       </c>
       <c r="I15">
         <v>100</v>
@@ -3138,11 +3138,11 @@
       </c>
       <c r="G16" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>HELPME</v>
       </c>
       <c r="H16" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H16" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Depressing</v>
+        <v>WeLostThem</v>
       </c>
       <c r="I16">
         <v>200</v>
@@ -3178,11 +3178,11 @@
       </c>
       <c r="F17" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F17" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>God'sPlan</v>
       </c>
       <c r="G17" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G17" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>WeLostThem</v>
       </c>
       <c r="H17" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H17" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -3222,15 +3222,15 @@
       </c>
       <c r="F18" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F18" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="G18" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="H18" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H18" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="I18">
         <v>350</v>
@@ -3266,15 +3266,15 @@
       </c>
       <c r="F19" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F19" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>LONGWaitTimes</v>
       </c>
       <c r="G19" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>CrapStaff</v>
       </c>
       <c r="H19" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H19" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="I19">
         <v>250</v>
@@ -3310,15 +3310,15 @@
       </c>
       <c r="F20" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F20" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="G20" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>ALWAYSSupport</v>
       </c>
       <c r="H20" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H20" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>CommunityBuild</v>
+        <v>ALWAYSSupport</v>
       </c>
       <c r="I20">
         <v>75</v>
@@ -3354,15 +3354,15 @@
       </c>
       <c r="F21" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F21" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="G21" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="H21" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H21" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="I21">
         <v>50</v>
@@ -3398,15 +3398,15 @@
       </c>
       <c r="F22" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F22" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="G22" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="H22" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H22" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="I22">
         <v>150</v>
@@ -3442,15 +3442,15 @@
       </c>
       <c r="F23" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F23" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>Desperate</v>
       </c>
       <c r="G23" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="H23" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H23" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>Outcast</v>
       </c>
       <c r="I23">
         <v>200</v>
@@ -3486,15 +3486,15 @@
       </c>
       <c r="F24" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F24" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="G24" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G24" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>OurLastHope</v>
       </c>
       <c r="H24" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H24" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="I24">
         <v>400</v>
@@ -3530,15 +3530,15 @@
       </c>
       <c r="F25" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F25" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="G25" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G25" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>OurLastHope</v>
       </c>
       <c r="H25" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H25" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="I25">
         <v>150</v>
@@ -3574,7 +3574,7 @@
       </c>
       <c r="F26" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F26" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>InGoodHands</v>
       </c>
       <c r="G26" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G26" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="H26" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H26" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v>RepeatElection</v>
       </c>
       <c r="I26">
         <v>75</v>
@@ -3618,15 +3618,15 @@
       </c>
       <c r="F27" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F27" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="G27" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G27" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>RepeatElection</v>
       </c>
       <c r="H27" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H27" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v>InGoodHands</v>
       </c>
       <c r="I27">
         <v>50</v>
@@ -3662,15 +3662,15 @@
       </c>
       <c r="F28" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F28" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>WhatAJoke</v>
       </c>
       <c r="G28" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G28" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="H28" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H28" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="I28">
         <v>100</v>
@@ -3706,7 +3706,7 @@
       </c>
       <c r="F29" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F29" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="G29" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G29" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="H29" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H29" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>I'maSitDown</v>
       </c>
       <c r="I29">
         <v>125</v>
@@ -3750,15 +3750,15 @@
       </c>
       <c r="F30" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F30" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RiotTIME</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="G30" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G30" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="H30" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H30" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="I30">
         <v>200</v>
@@ -3794,15 +3794,15 @@
       </c>
       <c r="F31" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F31" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>ToTheTorches!</v>
       </c>
       <c r="G31" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G31" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="H31" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H31" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>RiotTIME</v>
       </c>
       <c r="I31">
         <v>125</v>
@@ -3842,11 +3842,11 @@
       </c>
       <c r="G32" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G32" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>Hero</v>
       </c>
       <c r="H32" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H32" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FightBackTeam!</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="I32">
         <v>75</v>
@@ -3882,15 +3882,15 @@
       </c>
       <c r="F33" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F33" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>Justified!</v>
       </c>
       <c r="G33" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G33" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>Justice</v>
       </c>
       <c r="H33" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H33" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>BeSafe</v>
       </c>
       <c r="I33">
         <v>100</v>
@@ -3926,15 +3926,15 @@
       </c>
       <c r="F34" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F34" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>FreeThem</v>
       </c>
       <c r="G34" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G34" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>TooSoon</v>
       </c>
       <c r="H34" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H34" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>FreeThem</v>
       </c>
       <c r="I34">
         <v>225</v>
@@ -3970,7 +3970,7 @@
       </c>
       <c r="F35" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F35" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>Pathetic</v>
       </c>
       <c r="G35" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G35" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -3978,7 +3978,7 @@
       </c>
       <c r="H35" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H35" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>SoTragic</v>
       </c>
       <c r="I35">
         <v>175</v>
@@ -4014,15 +4014,15 @@
       </c>
       <c r="F36" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F36" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="G36" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G36" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>DeathCollection</v>
       </c>
       <c r="H36" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H36" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>PaybackTime</v>
       </c>
       <c r="I36">
         <v>325</v>
@@ -4058,15 +4058,15 @@
       </c>
       <c r="F37" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F37" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>PaybackTime</v>
       </c>
       <c r="G37" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G37" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="H37" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H37" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>DeathCollection</v>
       </c>
       <c r="I37">
         <v>200</v>
@@ -4102,15 +4102,15 @@
       </c>
       <c r="F38" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F38" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>100Sober</v>
+        <v>ThankGod</v>
       </c>
       <c r="G38" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G38" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>ThankGod</v>
       </c>
       <c r="H38" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H38" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>100Sober</v>
       </c>
       <c r="I38">
         <v>75</v>
@@ -4146,7 +4146,7 @@
       </c>
       <c r="F39" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F39" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>Recovered:)</v>
       </c>
       <c r="G39" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G39" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -4154,7 +4154,7 @@
       </c>
       <c r="H39" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H39" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>100Sober</v>
+        <v>ThankGod</v>
       </c>
       <c r="I39">
         <v>100</v>
@@ -4190,15 +4190,15 @@
       </c>
       <c r="F40" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F40" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>I'mSoLost</v>
       </c>
       <c r="G40" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G40" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>HardTimes</v>
       </c>
       <c r="H40" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H40" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>Drained</v>
       </c>
       <c r="I40">
         <v>200</v>
@@ -4238,11 +4238,11 @@
       </c>
       <c r="G41" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G41" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>HELPME</v>
       </c>
       <c r="H41" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H41" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>WeLostThem</v>
       </c>
       <c r="I41">
         <v>175</v>
@@ -4282,11 +4282,11 @@
       </c>
       <c r="G42" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G42" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="H42" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H42" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="I42">
         <v>350</v>
@@ -4326,11 +4326,11 @@
       </c>
       <c r="G43" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G43" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="H43" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H43" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>CrapStaff</v>
       </c>
       <c r="I43">
         <v>250</v>
@@ -4366,15 +4366,15 @@
       </c>
       <c r="F44" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F44" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="G44" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G44" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>ALWAYSSupport</v>
       </c>
       <c r="H44" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H44" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="I44">
         <v>75</v>
@@ -4410,11 +4410,11 @@
       </c>
       <c r="F45" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F45" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>ALWAYSSupport</v>
       </c>
       <c r="G45" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G45" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="H45" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H45" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -4458,11 +4458,11 @@
       </c>
       <c r="G46" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G46" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="H46" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H46" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>Outcast</v>
       </c>
       <c r="I46">
         <v>150</v>
@@ -4502,11 +4502,11 @@
       </c>
       <c r="G47" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G47" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="H47" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H47" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>Desperate</v>
       </c>
       <c r="I47">
         <v>200</v>
@@ -4542,15 +4542,15 @@
       </c>
       <c r="F48" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F48" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="G48" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G48" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="H48" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H48" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="I48">
         <v>400</v>
@@ -4586,15 +4586,15 @@
       </c>
       <c r="F49" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F49" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="G49" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G49" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>Messiah</v>
       </c>
       <c r="H49" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H49" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="I49">
         <v>150</v>
@@ -4630,15 +4630,15 @@
       </c>
       <c r="F50" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F50" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>InGoodHands</v>
       </c>
       <c r="G50" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G50" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>ReElect!!!</v>
       </c>
       <c r="H50" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H50" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>InGoodHands</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="I50">
         <v>75</v>
@@ -4674,11 +4674,11 @@
       </c>
       <c r="F51" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F51" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>InGoodHands</v>
       </c>
       <c r="G51" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G51" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>People'sVoice</v>
+        <v>ReElect!!!</v>
       </c>
       <c r="H51" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H51" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -4718,7 +4718,7 @@
       </c>
       <c r="F52" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F52" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="G52" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G52" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -4726,7 +4726,7 @@
       </c>
       <c r="H52" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H52" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>ItsOver</v>
       </c>
       <c r="I52">
         <v>100</v>
@@ -4762,15 +4762,15 @@
       </c>
       <c r="F53" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F53" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="G53" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G53" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="H53" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H53" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NoFaith</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="I53">
         <v>125</v>
@@ -4806,15 +4806,15 @@
       </c>
       <c r="F54" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F54" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>CoupDeTahhh</v>
+        <v>RaidingNight</v>
       </c>
       <c r="G54" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G54" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>RiotTIME</v>
       </c>
       <c r="H54" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H54" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="I54">
         <v>200</v>
@@ -4850,15 +4850,15 @@
       </c>
       <c r="F55" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F55" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="G55" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G55" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="H55" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H55" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="I55">
         <v>125</v>
@@ -4894,11 +4894,11 @@
       </c>
       <c r="F56" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F56" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="G56" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G56" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>ComeTogether!!</v>
       </c>
       <c r="H56" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H56" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -4938,15 +4938,15 @@
       </c>
       <c r="F57" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F57" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>Justice</v>
       </c>
       <c r="G57" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G57" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>ComeTogether!!</v>
       </c>
       <c r="H57" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H57" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>StrongerTogether</v>
       </c>
       <c r="I57">
         <v>100</v>
@@ -4982,15 +4982,15 @@
       </c>
       <c r="F58" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F58" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>FreeThem</v>
       </c>
       <c r="G58" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G58" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="H58" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H58" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="I58">
         <v>225</v>
@@ -5026,15 +5026,15 @@
       </c>
       <c r="F59" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F59" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>PrayForThem</v>
       </c>
       <c r="G59" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G59" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>TooSoon</v>
       </c>
       <c r="H59" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H59" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>SoTragic</v>
       </c>
       <c r="I59">
         <v>175</v>
@@ -5070,7 +5070,7 @@
       </c>
       <c r="F60" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F60" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>DeathCollection</v>
+        <v>Despicable!</v>
       </c>
       <c r="G60" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G60" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -5114,15 +5114,15 @@
       </c>
       <c r="F61" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F61" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>DeathCollection</v>
       </c>
       <c r="G61" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G61" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>DeathCollection</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="H61" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H61" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>PaybackTime</v>
       </c>
       <c r="I61">
         <v>200</v>
@@ -5158,15 +5158,15 @@
       </c>
       <c r="F62" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F62" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="G62" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G62" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>Recovered:)</v>
       </c>
       <c r="H62" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H62" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>100Sober</v>
       </c>
       <c r="I62">
         <v>75</v>
@@ -5206,11 +5206,11 @@
       </c>
       <c r="G63" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G63" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Hugs&amp;Kisses</v>
+        <v>BackToUs</v>
       </c>
       <c r="H63" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H63" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="I63">
         <v>100</v>
@@ -5246,15 +5246,15 @@
       </c>
       <c r="F64" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F64" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>Drained</v>
       </c>
       <c r="G64" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G64" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>Depressing</v>
       </c>
       <c r="H64" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H64" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>Drained</v>
       </c>
       <c r="I64">
         <v>200</v>
@@ -5290,15 +5290,15 @@
       </c>
       <c r="F65" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F65" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>Drained</v>
       </c>
       <c r="G65" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G65" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HELPME</v>
+        <v>HardTimes</v>
       </c>
       <c r="H65" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H65" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>HELPME</v>
       </c>
       <c r="I65">
         <v>175</v>
@@ -5334,15 +5334,15 @@
       </c>
       <c r="F66" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F66" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="G66" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G66" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="H66" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H66" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>CrapStaff</v>
       </c>
       <c r="I66">
         <v>350</v>
@@ -5378,15 +5378,15 @@
       </c>
       <c r="F67" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F67" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="G67" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G67" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="H67" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H67" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="I67">
         <v>250</v>
@@ -5422,11 +5422,11 @@
       </c>
       <c r="F68" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F68" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>CommunityBuild</v>
+        <v>WEStrong</v>
       </c>
       <c r="G68" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G68" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="H68" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H68" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -5466,7 +5466,7 @@
       </c>
       <c r="F69" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F69" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="G69" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G69" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -5474,7 +5474,7 @@
       </c>
       <c r="H69" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H69" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="I69">
         <v>50</v>
@@ -5514,11 +5514,11 @@
       </c>
       <c r="G70" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G70" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>SplitUp</v>
       </c>
       <c r="H70" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H70" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>Desperate</v>
       </c>
       <c r="I70">
         <v>150</v>
@@ -5554,15 +5554,15 @@
       </c>
       <c r="F71" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F71" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="G71" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G71" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WeNeedChange</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="H71" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H71" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="I71">
         <v>200</v>
@@ -5598,15 +5598,15 @@
       </c>
       <c r="F72" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F72" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="G72" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G72" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="H72" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H72" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="I72">
         <v>400</v>
@@ -5642,7 +5642,7 @@
       </c>
       <c r="F73" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F73" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>Messiah</v>
       </c>
       <c r="G73" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G73" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -5650,7 +5650,7 @@
       </c>
       <c r="H73" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H73" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="I73">
         <v>150</v>
@@ -5686,7 +5686,7 @@
       </c>
       <c r="F74" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F74" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v>ReElect!!!</v>
       </c>
       <c r="G74" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G74" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -5730,15 +5730,15 @@
       </c>
       <c r="F75" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F75" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v>RepeatElection</v>
       </c>
       <c r="G75" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G75" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>KeepThemIN!</v>
+        <v>RepeatElection</v>
       </c>
       <c r="H75" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H75" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="I75">
         <v>50</v>
@@ -5774,15 +5774,15 @@
       </c>
       <c r="F76" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F76" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="G76" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G76" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NoFaith</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="H76" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H76" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="I76">
         <v>100</v>
@@ -5822,11 +5822,11 @@
       </c>
       <c r="G77" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G77" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="H77" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H77" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>NoFaith</v>
       </c>
       <c r="I77">
         <v>125</v>
@@ -5862,15 +5862,15 @@
       </c>
       <c r="F78" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F78" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>ToTheTorches!</v>
       </c>
       <c r="G78" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G78" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>RaidingNight</v>
       </c>
       <c r="H78" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H78" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="I78">
         <v>200</v>
@@ -5906,15 +5906,15 @@
       </c>
       <c r="F79" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F79" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="G79" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G79" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>CoupDeTahhh</v>
+        <v>RiotTIME</v>
       </c>
       <c r="H79" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H79" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="I79">
         <v>125</v>
@@ -5950,15 +5950,15 @@
       </c>
       <c r="F80" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F80" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>Justified!</v>
       </c>
       <c r="G80" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G80" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>Justice</v>
       </c>
       <c r="H80" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H80" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>Justified!</v>
       </c>
       <c r="I80">
         <v>75</v>
@@ -5994,15 +5994,15 @@
       </c>
       <c r="F81" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F81" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>Justified!</v>
       </c>
       <c r="G81" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G81" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="H81" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H81" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>Justified!</v>
       </c>
       <c r="I81">
         <v>100</v>
@@ -6038,15 +6038,15 @@
       </c>
       <c r="F82" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F82" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>SoTragic</v>
       </c>
       <c r="G82" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G82" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>Pathetic</v>
       </c>
       <c r="H82" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H82" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>TooSoon</v>
       </c>
       <c r="I82">
         <v>225</v>
@@ -6082,15 +6082,15 @@
       </c>
       <c r="F83" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F83" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>SoTragic</v>
       </c>
       <c r="G83" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G83" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>WhatAShame</v>
       </c>
       <c r="H83" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H83" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FreeThem</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="I83">
         <v>175</v>
@@ -6126,15 +6126,15 @@
       </c>
       <c r="F84" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F84" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="G84" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G84" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>DeathCollection</v>
+        <v>PaybackTime</v>
       </c>
       <c r="H84" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H84" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="I84">
         <v>325</v>
@@ -6170,15 +6170,15 @@
       </c>
       <c r="F85" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F85" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="G85" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G85" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>DeathCollection</v>
+        <v>PaybackTime</v>
       </c>
       <c r="H85" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H85" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="I85">
         <v>200</v>
@@ -6214,7 +6214,7 @@
       </c>
       <c r="F86" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F86" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>ThankGod</v>
       </c>
       <c r="G86" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G86" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -6222,7 +6222,7 @@
       </c>
       <c r="H86" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H86" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="I86">
         <v>75</v>
@@ -6258,15 +6258,15 @@
       </c>
       <c r="F87" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F87" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="G87" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G87" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>MadeIt</v>
       </c>
       <c r="H87" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H87" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>100Sober</v>
       </c>
       <c r="I87">
         <v>100</v>
@@ -6302,15 +6302,15 @@
       </c>
       <c r="F88" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F88" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>Depressing</v>
       </c>
       <c r="G88" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G88" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HELPME</v>
+        <v>God'sPlan</v>
       </c>
       <c r="H88" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H88" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="I88">
         <v>200</v>
@@ -6346,15 +6346,15 @@
       </c>
       <c r="F89" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F89" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>HardTimes</v>
       </c>
       <c r="G89" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G89" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>WeLostThem</v>
       </c>
       <c r="H89" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H89" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>Drained</v>
       </c>
       <c r="I89">
         <v>175</v>
@@ -6390,15 +6390,15 @@
       </c>
       <c r="F90" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F90" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>LONGWaitTimes</v>
       </c>
       <c r="G90" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G90" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="H90" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H90" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="I90">
         <v>350</v>
@@ -6434,15 +6434,15 @@
       </c>
       <c r="F91" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F91" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="G91" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G91" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="H91" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H91" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="I91">
         <v>250</v>
@@ -6478,15 +6478,15 @@
       </c>
       <c r="F92" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F92" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>WEStrong</v>
       </c>
       <c r="G92" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G92" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>WEStrong</v>
       </c>
       <c r="H92" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H92" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WEStrong</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="I92">
         <v>75</v>
@@ -6522,15 +6522,15 @@
       </c>
       <c r="F93" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F93" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="G93" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G93" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="H93" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H93" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>WEStrong</v>
       </c>
       <c r="I93">
         <v>50</v>
@@ -6566,7 +6566,7 @@
       </c>
       <c r="F94" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F94" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WeNeedChange</v>
+        <v>SplitUp</v>
       </c>
       <c r="G94" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G94" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -6574,7 +6574,7 @@
       </c>
       <c r="H94" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H94" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="I94">
         <v>150</v>
@@ -6610,15 +6610,15 @@
       </c>
       <c r="F95" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F95" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="G95" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G95" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="H95" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H95" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>SplitUp</v>
       </c>
       <c r="I95">
         <v>200</v>
@@ -6654,15 +6654,15 @@
       </c>
       <c r="F96" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F96" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="G96" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G96" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="H96" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H96" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="I96">
         <v>400</v>
@@ -6698,15 +6698,15 @@
       </c>
       <c r="F97" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F97" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="G97" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G97" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="H97" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H97" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>NecessaryEvil</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="I97">
         <v>150</v>
@@ -6742,7 +6742,7 @@
       </c>
       <c r="F98" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F98" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v xml:space="preserve">Saviours </v>
       </c>
       <c r="G98" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G98" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -6750,7 +6750,7 @@
       </c>
       <c r="H98" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H98" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>InGoodHands</v>
       </c>
       <c r="I98">
         <v>75</v>
@@ -6786,11 +6786,11 @@
       </c>
       <c r="F99" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F99" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="G99" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G99" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="H99" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H99" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -6830,7 +6830,7 @@
       </c>
       <c r="F100" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F100" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="G100" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G100" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="H100" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H100" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="I100">
         <v>100</v>
@@ -6878,11 +6878,11 @@
       </c>
       <c r="G101" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G101" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="H101" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H101" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsDownhill</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="I101">
         <v>125</v>
@@ -6918,15 +6918,15 @@
       </c>
       <c r="F102" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F102" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="G102" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G102" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>RaidingNight</v>
       </c>
       <c r="H102" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H102" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="I102">
         <v>200</v>
@@ -6970,7 +6970,7 @@
       </c>
       <c r="H103" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H103" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>RiotTIME</v>
       </c>
       <c r="I103">
         <v>125</v>
@@ -7006,15 +7006,15 @@
       </c>
       <c r="F104" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F104" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>ComeTogether!!</v>
       </c>
       <c r="G104" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G104" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>ComeTogether!!</v>
       </c>
       <c r="H104" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H104" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>BeSafe</v>
       </c>
       <c r="I104">
         <v>75</v>
@@ -7050,15 +7050,15 @@
       </c>
       <c r="F105" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F105" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>Justified!</v>
       </c>
       <c r="G105" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G105" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>Justice</v>
       </c>
       <c r="H105" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H105" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>Justified!</v>
       </c>
       <c r="I105">
         <v>100</v>
@@ -7094,15 +7094,15 @@
       </c>
       <c r="F106" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F106" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>FreeThem</v>
       </c>
       <c r="G106" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G106" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>FreeThem</v>
       </c>
       <c r="H106" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H106" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>Lowlife</v>
       </c>
       <c r="I106">
         <v>225</v>
@@ -7138,15 +7138,15 @@
       </c>
       <c r="F107" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F107" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>WhatAShame</v>
       </c>
       <c r="G107" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G107" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="H107" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H107" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>TooSoon</v>
       </c>
       <c r="I107">
         <v>175</v>
@@ -7182,15 +7182,15 @@
       </c>
       <c r="F108" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F108" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="G108" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G108" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>Despicable!</v>
       </c>
       <c r="H108" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H108" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>AskingForIt</v>
       </c>
       <c r="I108">
         <v>325</v>
@@ -7230,11 +7230,11 @@
       </c>
       <c r="G109" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G109" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>Despicable!</v>
       </c>
       <c r="H109" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H109" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>PaybackTime</v>
       </c>
       <c r="I109">
         <v>200</v>
@@ -7270,15 +7270,15 @@
       </c>
       <c r="F110" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F110" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Hugs&amp;Kisses</v>
+        <v>100Sober</v>
       </c>
       <c r="G110" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G110" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>100Sober</v>
       </c>
       <c r="H110" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H110" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>BackToUs</v>
       </c>
       <c r="I110">
         <v>75</v>
@@ -7314,15 +7314,15 @@
       </c>
       <c r="F111" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F111" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>MadeIt</v>
       </c>
       <c r="G111" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G111" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="H111" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H111" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>BestWishes</v>
       </c>
       <c r="I111">
         <v>100</v>
@@ -7358,15 +7358,15 @@
       </c>
       <c r="F112" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F112" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>Depressing</v>
       </c>
       <c r="G112" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G112" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>HELPME</v>
       </c>
       <c r="H112" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H112" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>Drained</v>
       </c>
       <c r="I112">
         <v>200</v>
@@ -7402,15 +7402,15 @@
       </c>
       <c r="F113" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F113" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>HardTimes</v>
       </c>
       <c r="G113" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G113" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>God'sPlan</v>
       </c>
       <c r="H113" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H113" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>Drained</v>
       </c>
       <c r="I113">
         <v>175</v>
@@ -7446,15 +7446,15 @@
       </c>
       <c r="F114" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F114" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>Refund</v>
       </c>
       <c r="G114" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G114" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="H114" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H114" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="I114">
         <v>350</v>
@@ -7490,15 +7490,15 @@
       </c>
       <c r="F115" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F115" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Refund</v>
+        <v>CrapStaff</v>
       </c>
       <c r="G115" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G115" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>CrapStaff</v>
       </c>
       <c r="H115" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H115" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>Refund</v>
       </c>
       <c r="I115">
         <v>250</v>
@@ -7534,15 +7534,15 @@
       </c>
       <c r="F116" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F116" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="G116" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G116" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="H116" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H116" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="I116">
         <v>75</v>
@@ -7578,15 +7578,15 @@
       </c>
       <c r="F117" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F117" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>WEStrong</v>
       </c>
       <c r="G117" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G117" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="H117" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H117" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="I117">
         <v>50</v>
@@ -7622,7 +7622,7 @@
       </c>
       <c r="F118" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F118" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="G118" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G118" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -7630,7 +7630,7 @@
       </c>
       <c r="H118" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H118" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="I118">
         <v>150</v>
@@ -7666,15 +7666,15 @@
       </c>
       <c r="F119" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F119" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="G119" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G119" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WeNeedChange</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="H119" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H119" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="I119">
         <v>200</v>
@@ -7710,15 +7710,15 @@
       </c>
       <c r="F120" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F120" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>OurLastHope</v>
       </c>
       <c r="G120" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G120" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="H120" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H120" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>NecessaryEvil</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="I120">
         <v>400</v>
@@ -7754,11 +7754,11 @@
       </c>
       <c r="F121" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F121" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="G121" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G121" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>Messiah</v>
       </c>
       <c r="H121" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H121" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -7798,15 +7798,15 @@
       </c>
       <c r="F122" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F122" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v>People'sVoice</v>
       </c>
       <c r="G122" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G122" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>KeepThemIN!</v>
+        <v xml:space="preserve">Saviours </v>
       </c>
       <c r="H122" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H122" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>VoteAgain</v>
       </c>
       <c r="I122">
         <v>75</v>
@@ -7846,11 +7846,11 @@
       </c>
       <c r="G123" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G123" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>People'sVoice</v>
       </c>
       <c r="H123" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H123" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>InGoodHands</v>
       </c>
       <c r="I123">
         <v>50</v>
@@ -7890,11 +7890,11 @@
       </c>
       <c r="G124" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G124" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>NoFaith</v>
       </c>
       <c r="H124" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H124" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NoFaith</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="I124">
         <v>100</v>
@@ -7930,15 +7930,15 @@
       </c>
       <c r="F125" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F125" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="G125" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G125" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>ItsOver</v>
       </c>
       <c r="H125" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H125" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="I125">
         <v>125</v>
@@ -7978,11 +7978,11 @@
       </c>
       <c r="G126" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G126" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="H126" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H126" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>ToTheTorches!</v>
       </c>
       <c r="I126">
         <v>200</v>
@@ -8018,15 +8018,15 @@
       </c>
       <c r="F127" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F127" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>RiotTIME</v>
       </c>
       <c r="G127" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G127" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>RiotTIME</v>
       </c>
       <c r="H127" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H127" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RaidingNight</v>
+        <v>BurnItDOWN</v>
       </c>
       <c r="I127">
         <v>125</v>
@@ -8062,15 +8062,15 @@
       </c>
       <c r="F128" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F128" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FightBackTeam!</v>
+        <v>Hero</v>
       </c>
       <c r="G128" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G128" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>Hero</v>
       </c>
       <c r="H128" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H128" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>StrongerTogether</v>
       </c>
       <c r="I128">
         <v>75</v>
@@ -8154,11 +8154,11 @@
       </c>
       <c r="G130" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G130" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>FreeThem</v>
       </c>
       <c r="H130" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H130" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>WhatAShame</v>
+        <v>FreeThem</v>
       </c>
       <c r="I130">
         <v>225</v>
@@ -8198,11 +8198,11 @@
       </c>
       <c r="G131" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G131" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>TooSoon</v>
       </c>
       <c r="H131" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H131" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PrayForThem</v>
+        <v>SoTragic</v>
       </c>
       <c r="I131">
         <v>175</v>
@@ -8238,15 +8238,15 @@
       </c>
       <c r="F132" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F132" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="G132" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G132" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="H132" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H132" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>DeathCollection</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="I132">
         <v>325</v>
@@ -8282,15 +8282,15 @@
       </c>
       <c r="F133" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F133" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>Despicable!</v>
       </c>
       <c r="G133" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G133" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="H133" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H133" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>AskingForIt</v>
       </c>
       <c r="I133">
         <v>200</v>
@@ -8326,15 +8326,15 @@
       </c>
       <c r="F134" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F134" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="G134" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G134" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>BestWishes</v>
       </c>
       <c r="H134" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H134" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>BestWishes</v>
       </c>
       <c r="I134">
         <v>75</v>
@@ -8374,11 +8374,11 @@
       </c>
       <c r="G135" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G135" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BestWishes</v>
+        <v>Recovered:)</v>
       </c>
       <c r="H135" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H135" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Recovered:)</v>
+        <v>100Sober</v>
       </c>
       <c r="I135">
         <v>100</v>
@@ -8418,11 +8418,11 @@
       </c>
       <c r="G136" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G136" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>HELPME</v>
       </c>
       <c r="H136" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H136" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="I136">
         <v>200</v>
@@ -8462,11 +8462,11 @@
       </c>
       <c r="G137" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G137" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>I'mSoLost</v>
       </c>
       <c r="H137" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H137" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HELPME</v>
+        <v>Depressing</v>
       </c>
       <c r="I137">
         <v>175</v>
@@ -8502,15 +8502,15 @@
       </c>
       <c r="F138" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F138" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="G138" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G138" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>Refund</v>
       </c>
       <c r="H138" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H138" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>LONGWaitTimes</v>
       </c>
       <c r="I138">
         <v>350</v>
@@ -8546,15 +8546,15 @@
       </c>
       <c r="F139" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F139" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="G139" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G139" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="H139" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H139" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="I139">
         <v>250</v>
@@ -8590,15 +8590,15 @@
       </c>
       <c r="F140" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F140" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="G140" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G140" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>WEStrong</v>
       </c>
       <c r="H140" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H140" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>CommunityBuild</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="I140">
         <v>75</v>
@@ -8634,7 +8634,7 @@
       </c>
       <c r="F141" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F141" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="G141" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G141" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -8642,7 +8642,7 @@
       </c>
       <c r="H141" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H141" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="I141">
         <v>50</v>
@@ -8678,15 +8678,15 @@
       </c>
       <c r="F142" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F142" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>Desperate</v>
       </c>
       <c r="G142" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G142" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="H142" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H142" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>Outcast</v>
       </c>
       <c r="I142">
         <v>150</v>
@@ -8722,15 +8722,15 @@
       </c>
       <c r="F143" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F143" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>Desperate</v>
       </c>
       <c r="G143" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G143" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>Desperate</v>
       </c>
       <c r="H143" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H143" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>SplitUp</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="I143">
         <v>200</v>
@@ -8766,11 +8766,11 @@
       </c>
       <c r="F144" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F144" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="G144" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G144" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="H144" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H144" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -8810,15 +8810,15 @@
       </c>
       <c r="F145" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F145" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="G145" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G145" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurLastHope</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="H145" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H145" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="I145">
         <v>150</v>
@@ -8854,7 +8854,7 @@
       </c>
       <c r="F146" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F146" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>People'sVoice</v>
       </c>
       <c r="G146" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G146" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -8862,7 +8862,7 @@
       </c>
       <c r="H146" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H146" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>People'sVoice</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="I146">
         <v>75</v>
@@ -8898,11 +8898,11 @@
       </c>
       <c r="F147" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F147" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>RepeatElection</v>
       </c>
       <c r="G147" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G147" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>GetsThingsDone</v>
       </c>
       <c r="H147" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H147" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -8942,15 +8942,15 @@
       </c>
       <c r="F148" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F148" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>NotAgainnnn</v>
       </c>
       <c r="G148" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G148" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NoFaith</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="H148" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H148" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>I'maSitDown</v>
       </c>
       <c r="I148">
         <v>100</v>
@@ -8986,15 +8986,15 @@
       </c>
       <c r="F149" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F149" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>WhatAJoke</v>
       </c>
       <c r="G149" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G149" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="H149" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H149" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>WhatAJoke</v>
       </c>
       <c r="I149">
         <v>125</v>
@@ -9030,15 +9030,15 @@
       </c>
       <c r="F150" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F150" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="G150" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G150" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>CoupDeTahhh</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="H150" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H150" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Pitchforks!!!</v>
+        <v>RiotTIME</v>
       </c>
       <c r="I150">
         <v>200</v>
@@ -9074,15 +9074,15 @@
       </c>
       <c r="F151" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F151" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>RaidingNight</v>
       </c>
       <c r="G151" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G151" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>BurnItDOWN</v>
       </c>
       <c r="H151" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H151" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>CoupDeTahhh</v>
+        <v>RiotTIME</v>
       </c>
       <c r="I151">
         <v>125</v>
@@ -9118,15 +9118,15 @@
       </c>
       <c r="F152" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F152" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>ComeTogether!!</v>
       </c>
       <c r="G152" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G152" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>BeSafe</v>
       </c>
       <c r="H152" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H152" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>Hero</v>
       </c>
       <c r="I152">
         <v>75</v>
@@ -9162,15 +9162,15 @@
       </c>
       <c r="F153" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F153" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>Justice</v>
       </c>
       <c r="G153" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G153" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>ComeTogether!!</v>
+        <v>Justified!</v>
       </c>
       <c r="H153" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H153" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="I153">
         <v>100</v>
@@ -9206,15 +9206,15 @@
       </c>
       <c r="F154" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F154" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>FreeThem</v>
       </c>
       <c r="G154" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G154" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>Lowlife</v>
       </c>
       <c r="H154" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H154" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>Pathetic</v>
       </c>
       <c r="I154">
         <v>225</v>
@@ -9250,15 +9250,15 @@
       </c>
       <c r="F155" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F155" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>Lowlife</v>
       </c>
       <c r="G155" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G155" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>GodLeftChat</v>
+        <v>FreeThem</v>
       </c>
       <c r="H155" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H155" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TooSoon</v>
+        <v>FreeThem</v>
       </c>
       <c r="I155">
         <v>175</v>
@@ -9294,15 +9294,15 @@
       </c>
       <c r="F156" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F156" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>DeathCollection</v>
       </c>
       <c r="G156" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G156" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>Despicable!</v>
       </c>
       <c r="H156" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H156" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>AskingForIt</v>
       </c>
       <c r="I156">
         <v>325</v>
@@ -9338,15 +9338,15 @@
       </c>
       <c r="F157" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F157" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>PaybackTime</v>
       </c>
       <c r="G157" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G157" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>Despicable!</v>
       </c>
       <c r="H157" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H157" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>Despicable!</v>
       </c>
       <c r="I157">
         <v>200</v>
@@ -9382,15 +9382,15 @@
       </c>
       <c r="F158" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F158" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>BackToUs</v>
       </c>
       <c r="G158" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G158" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Hugs&amp;Kisses</v>
+        <v>100Sober</v>
       </c>
       <c r="H158" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H158" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="I158">
         <v>75</v>
@@ -9426,15 +9426,15 @@
       </c>
       <c r="F159" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F159" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>BestWishes</v>
       </c>
       <c r="G159" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G159" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Hugs&amp;Kisses</v>
+        <v>ThankGod</v>
       </c>
       <c r="H159" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H159" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>BestWishes</v>
       </c>
       <c r="I159">
         <v>100</v>
@@ -9470,7 +9470,7 @@
       </c>
       <c r="F160" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F160" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>God'sPlan</v>
       </c>
       <c r="G160" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G160" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -9478,7 +9478,7 @@
       </c>
       <c r="H160" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H160" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>I'mSoLost</v>
       </c>
       <c r="I160">
         <v>200</v>
@@ -9514,15 +9514,15 @@
       </c>
       <c r="F161" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F161" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HardTimes</v>
+        <v>Depressing</v>
       </c>
       <c r="G161" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G161" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="H161" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H161" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>God'sPlan</v>
       </c>
       <c r="I161">
         <v>175</v>
@@ -9566,7 +9566,7 @@
       </c>
       <c r="H162" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H162" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="I162">
         <v>350</v>
@@ -9602,15 +9602,15 @@
       </c>
       <c r="F163" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F163" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="G163" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G163" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>CrapStaff</v>
       </c>
       <c r="H163" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H163" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="I163">
         <v>250</v>
@@ -9646,15 +9646,15 @@
       </c>
       <c r="F164" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F164" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="G164" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G164" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="H164" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H164" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="I164">
         <v>75</v>
@@ -9690,7 +9690,7 @@
       </c>
       <c r="F165" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F165" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WEStrong</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="G165" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G165" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -9698,7 +9698,7 @@
       </c>
       <c r="H165" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H165" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>ALWAYSSupport</v>
       </c>
       <c r="I165">
         <v>50</v>
@@ -9734,15 +9734,15 @@
       </c>
       <c r="F166" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F166" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WeNeedChange</v>
+        <v>Outcast</v>
       </c>
       <c r="G166" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G166" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>Desperate</v>
       </c>
       <c r="H166" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H166" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="I166">
         <v>150</v>
@@ -9778,7 +9778,7 @@
       </c>
       <c r="F167" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F167" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>SplitUp</v>
       </c>
       <c r="G167" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G167" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -9786,7 +9786,7 @@
       </c>
       <c r="H167" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H167" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="I167">
         <v>200</v>
@@ -9822,15 +9822,15 @@
       </c>
       <c r="F168" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F168" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="G168" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G168" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>Messiah</v>
       </c>
       <c r="H168" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H168" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>NecessaryEvil</v>
+        <v>Messiah</v>
       </c>
       <c r="I168">
         <v>400</v>
@@ -9866,15 +9866,15 @@
       </c>
       <c r="F169" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F169" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>OurLastHope</v>
       </c>
       <c r="G169" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G169" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="H169" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H169" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>OurLastHope</v>
       </c>
       <c r="I169">
         <v>150</v>
@@ -9910,11 +9910,11 @@
       </c>
       <c r="F170" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F170" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="G170" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G170" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v xml:space="preserve">Saviours </v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="H170" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H170" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -9954,15 +9954,15 @@
       </c>
       <c r="F171" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F171" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>People'sVoice</v>
       </c>
       <c r="G171" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G171" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>VoteAgain</v>
       </c>
       <c r="H171" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H171" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>People'sVoice</v>
+        <v>InGoodHands</v>
       </c>
       <c r="I171">
         <v>50</v>
@@ -9998,15 +9998,15 @@
       </c>
       <c r="F172" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F172" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>Where'sTioSammy</v>
       </c>
       <c r="G172" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G172" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WhatAJoke</v>
+        <v>ItsOver</v>
       </c>
       <c r="H172" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H172" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="I172">
         <v>100</v>
@@ -10042,15 +10042,15 @@
       </c>
       <c r="F173" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F173" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>WeAreDoomed</v>
+        <v>NoFaith</v>
       </c>
       <c r="G173" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G173" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>I'maSitDown</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="H173" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H173" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>WeAreDoomed</v>
       </c>
       <c r="I173">
         <v>125</v>
@@ -10086,15 +10086,15 @@
       </c>
       <c r="F174" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F174" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>BurnItDOWN</v>
       </c>
       <c r="G174" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G174" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>LeRevolution!</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="H174" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H174" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>CoupDeTahhh</v>
       </c>
       <c r="I174">
         <v>200</v>
@@ -10130,15 +10130,15 @@
       </c>
       <c r="F175" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F175" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="G175" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G175" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>RiotTIME</v>
       </c>
       <c r="H175" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H175" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>Pitchforks!!!</v>
       </c>
       <c r="I175">
         <v>125</v>
@@ -10178,11 +10178,11 @@
       </c>
       <c r="G176" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G176" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BeSafe</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="H176" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H176" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>StandUp!!!</v>
       </c>
       <c r="I176">
         <v>75</v>
@@ -10222,11 +10222,11 @@
       </c>
       <c r="G177" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G177" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>BeSafe</v>
       </c>
       <c r="H177" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H177" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Hero</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="I177">
         <v>100</v>
@@ -10262,15 +10262,15 @@
       </c>
       <c r="F178" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F178" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>GodLeftChat</v>
       </c>
       <c r="G178" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G178" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>WhatAShame</v>
       </c>
       <c r="H178" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H178" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FreeThem</v>
+        <v>Pathetic</v>
       </c>
       <c r="I178">
         <v>225</v>
@@ -10306,15 +10306,15 @@
       </c>
       <c r="F179" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F179" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>TooSoon</v>
       </c>
       <c r="G179" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G179" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FreeThem</v>
+        <v>WhatAShame</v>
       </c>
       <c r="H179" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H179" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FreeThem</v>
+        <v>Pathetic</v>
       </c>
       <c r="I179">
         <v>175</v>
@@ -10350,15 +10350,15 @@
       </c>
       <c r="F180" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F180" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>NoJustice!!!</v>
+        <v>PaybackTime</v>
       </c>
       <c r="G180" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G180" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>BetterOffDead</v>
+        <v>Despicable!</v>
       </c>
       <c r="H180" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H180" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Despicable!</v>
+        <v>NoJustice!!!</v>
       </c>
       <c r="I180">
         <v>325</v>
@@ -10394,15 +10394,15 @@
       </c>
       <c r="F181" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F181" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="G181" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G181" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>TakeEmDOWN!!!</v>
+        <v>AskingForIt</v>
       </c>
       <c r="H181" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H181" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>AskingForIt</v>
       </c>
       <c r="I181">
         <v>200</v>
@@ -10438,15 +10438,15 @@
       </c>
       <c r="F182" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F182" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>100Sober</v>
       </c>
       <c r="G182" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G182" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>Hugs&amp;Kisses</v>
       </c>
       <c r="H182" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H182" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>BestWishes</v>
       </c>
       <c r="I182">
         <v>75</v>
@@ -10482,15 +10482,15 @@
       </c>
       <c r="F183" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F183" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>ThankGod</v>
       </c>
       <c r="G183" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G183" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>BackToUs</v>
       </c>
       <c r="H183" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H183" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Safe&amp;Sound</v>
+        <v>BackToUs</v>
       </c>
       <c r="I183">
         <v>100</v>
@@ -10526,15 +10526,15 @@
       </c>
       <c r="F184" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F184" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Depressing</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="G184" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G184" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankYouAll</v>
+        <v>WeLostThem</v>
       </c>
       <c r="H184" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H184" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>God'sPlan</v>
+        <v>HardTimes</v>
       </c>
       <c r="I184">
         <v>200</v>
@@ -10570,15 +10570,15 @@
       </c>
       <c r="F185" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F185" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HELPME</v>
+        <v>Drained</v>
       </c>
       <c r="G185" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G185" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>HELPME</v>
+        <v>HardTimes</v>
       </c>
       <c r="H185" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H185" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Depressing</v>
+        <v>Drained</v>
       </c>
       <c r="I185">
         <v>175</v>
@@ -10614,15 +10614,15 @@
       </c>
       <c r="F186" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F186" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="G186" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G186" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>TaxedForThis?</v>
       </c>
       <c r="H186" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H186" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>LONGWaitTimes</v>
+        <v>Refund</v>
       </c>
       <c r="I186">
         <v>350</v>
@@ -10658,15 +10658,15 @@
       </c>
       <c r="F187" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F187" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>UnderStaffed!!</v>
       </c>
       <c r="G187" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G187" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrapStaff</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="H187" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H187" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>TaxedForThis?</v>
+        <v>CrappyHealthCare</v>
       </c>
       <c r="I187">
         <v>250</v>
@@ -10702,15 +10702,15 @@
       </c>
       <c r="F188" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F188" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="G188" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G188" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>CommunityBuild</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="H188" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H188" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WEStrong</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="I188">
         <v>75</v>
@@ -10746,15 +10746,15 @@
       </c>
       <c r="F189" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F189" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OpenMinded!</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="G189" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G189" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="H189" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H189" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>RallyTogether!</v>
+        <v>OpenMinded!</v>
       </c>
       <c r="I189">
         <v>50</v>
@@ -10790,15 +10790,15 @@
       </c>
       <c r="F190" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F190" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ItsTheOnlyWay</v>
+        <v>Outcast</v>
       </c>
       <c r="G190" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G190" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>SplitUp</v>
       </c>
       <c r="H190" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H190" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>ItsTheOnlyWay</v>
       </c>
       <c r="I190">
         <v>150</v>
@@ -10834,15 +10834,15 @@
       </c>
       <c r="F191" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F191" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AlwaysThem</v>
+        <v>SplitUp</v>
       </c>
       <c r="G191" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G191" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>WeNeedChange</v>
       </c>
       <c r="H191" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H191" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>SplitUp</v>
       </c>
       <c r="I191">
         <v>200</v>
@@ -10878,15 +10878,15 @@
       </c>
       <c r="F192" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F192" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>MessEmUP!!!</v>
       </c>
       <c r="G192" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G192" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>OurLastHope</v>
       </c>
       <c r="H192" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H192" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MessEmUP!!!</v>
+        <v>Divide&amp;CONQUER</v>
       </c>
       <c r="I192">
         <v>400</v>
@@ -10922,15 +10922,15 @@
       </c>
       <c r="F193" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F193" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="G193" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G193" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>MartyrUS!!</v>
+        <v>AgainstUS!!</v>
       </c>
       <c r="H193" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H193" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Divide&amp;CONQUER</v>
+        <v>Messiah</v>
       </c>
       <c r="I193">
         <v>150</v>
@@ -10966,15 +10966,15 @@
       </c>
       <c r="F194" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F194" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetsThingsDone</v>
+        <v>ReElect!!!</v>
       </c>
       <c r="G194" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G194" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>VoteAgain</v>
       </c>
       <c r="H194" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H194" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>VoteAgain</v>
+        <v>InGoodHands</v>
       </c>
       <c r="I194">
         <v>75</v>
@@ -11010,15 +11010,15 @@
       </c>
       <c r="F195" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F195" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>InGoodHands</v>
       </c>
       <c r="G195" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G195" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>RepeatElection</v>
+        <v>People'sVoice</v>
       </c>
       <c r="H195" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H195" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ReElect!!!</v>
+        <v>KeepThemIN!</v>
       </c>
       <c r="I195">
         <v>50</v>
@@ -11054,15 +11054,15 @@
       </c>
       <c r="F196" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F196" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NotAgainnnn</v>
+        <v>ItsDownhill</v>
       </c>
       <c r="G196" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G196" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>Where'sTioSammy</v>
+        <v>ItsOver</v>
       </c>
       <c r="H196" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H196" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NoFaith</v>
+        <v>ItsOver</v>
       </c>
       <c r="I196">
         <v>100</v>
@@ -11098,15 +11098,15 @@
       </c>
       <c r="F197" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F197" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NoFaith</v>
+        <v>WhatAJoke</v>
       </c>
       <c r="G197" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G197" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>NoFaith</v>
+        <v>ItsOver</v>
       </c>
       <c r="H197" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H197" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ItsOver</v>
+        <v>I'maSitDown</v>
       </c>
       <c r="I197">
         <v>125</v>
@@ -11142,11 +11142,11 @@
       </c>
       <c r="F198" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F198" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>BurnItDOWN</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="G198" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G198" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>RaidingNight</v>
       </c>
       <c r="H198" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H198" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -11186,11 +11186,11 @@
       </c>
       <c r="F199" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="F199" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>ToTheTorches!</v>
+        <v>GetEmOUT</v>
       </c>
       <c r="G199" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="G199" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
-        <v>GetEmOUT</v>
+        <v>LeRevolution!</v>
       </c>
       <c r="H199" s="8" t="str" cm="1">
         <f t="array" aca="1" ref="H199" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] = "Government", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$2:$B$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$2:$B$9)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$2:$C$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$2:$C$9)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$2:$D$9,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$2:$D$9)),1),Null))))</f>
@@ -11230,15 +11230,15 @@
       </c>
       <c r="F200" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F200" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justified!</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="G200" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G200" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StandUp!!!</v>
+        <v>FightBackTeam!</v>
       </c>
       <c r="H200" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H200" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>Justified!</v>
       </c>
       <c r="I200">
         <v>75</v>
@@ -11274,15 +11274,15 @@
       </c>
       <c r="F201" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F201" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>StrongerTogether</v>
+        <v>BeSafe</v>
       </c>
       <c r="G201" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G201" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>FightBackTeam!</v>
+        <v>Justice</v>
       </c>
       <c r="H201" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H201" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Justice</v>
+        <v>BeSafe</v>
       </c>
       <c r="I201">
         <v>100</v>
@@ -11322,11 +11322,11 @@
       </c>
       <c r="G202" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G202" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>SoTragic</v>
+        <v>Pathetic</v>
       </c>
       <c r="H202" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H202" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>TooSoon</v>
       </c>
       <c r="I202">
         <v>225</v>
@@ -11362,15 +11362,15 @@
       </c>
       <c r="F203" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F203" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Lowlife</v>
+        <v>WhatAShame</v>
       </c>
       <c r="G203" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G203" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>TooSoon</v>
       </c>
       <c r="H203" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H203" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Pathetic</v>
+        <v>PrayForThem</v>
       </c>
       <c r="I203">
         <v>175</v>
@@ -11406,11 +11406,11 @@
       </c>
       <c r="F204" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F204" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>DeathCollection</v>
+        <v>Eye-ForAn-Eye</v>
       </c>
       <c r="G204" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G204" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>DeathCollection</v>
+        <v>AskingForIt</v>
       </c>
       <c r="H204" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H204" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
@@ -11450,15 +11450,15 @@
       </c>
       <c r="F205" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F205" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>Eye-ForAn-Eye</v>
+        <v>TakeEmDOWN!!!</v>
       </c>
       <c r="G205" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G205" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>PaybackTime</v>
+        <v>AskingForIt</v>
       </c>
       <c r="H205" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H205" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Violence", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$10:$B$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$10:$B$17)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$10:$C$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$10:$C$17)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$10:$D$17,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$10:$D$17)),1),Null))))</f>
-        <v>AskingForIt</v>
+        <v>BetterOffDead</v>
       </c>
       <c r="I205">
         <v>200</v>
@@ -11498,11 +11498,11 @@
       </c>
       <c r="G206" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G206" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>ThankGod</v>
+        <v>100Sober</v>
       </c>
       <c r="H206" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H206" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>BackToUs</v>
+        <v>BestWishes</v>
       </c>
       <c r="I206">
         <v>75</v>
@@ -11538,11 +11538,11 @@
       </c>
       <c r="F207" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F207" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MadeIt</v>
+        <v>Safe&amp;Sound</v>
       </c>
       <c r="G207" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G207" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Hugs&amp;Kisses</v>
+        <v>Recovered:)</v>
       </c>
       <c r="H207" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H207" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
@@ -11582,15 +11582,15 @@
       </c>
       <c r="F208" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F208" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>WeLostThem</v>
+        <v>ThankYouAll</v>
       </c>
       <c r="G208" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G208" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>God'sPlan</v>
       </c>
       <c r="H208" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H208" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Depressing</v>
+        <v>HELPME</v>
       </c>
       <c r="I208">
         <v>200</v>
@@ -11630,11 +11630,11 @@
       </c>
       <c r="G209" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G209" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>Drained</v>
+        <v>Depressing</v>
       </c>
       <c r="H209" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H209" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>I'mSoLost</v>
+        <v>Depressing</v>
       </c>
       <c r="I209">
         <v>175</v>
@@ -11670,15 +11670,15 @@
       </c>
       <c r="F210" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F210" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>CrapStaff</v>
       </c>
       <c r="G210" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G210" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>CrapStaff</v>
       </c>
       <c r="H210" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H210" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>CrappyHealthCare</v>
+        <v>OverpaidIdiots</v>
       </c>
       <c r="I210">
         <v>350</v>
@@ -11714,15 +11714,15 @@
       </c>
       <c r="F211" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F211" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>OverpaidIdiots</v>
+        <v>Refund</v>
       </c>
       <c r="G211" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G211" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>UnderStaffed!!</v>
+        <v>MoneyWasted</v>
       </c>
       <c r="H211" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="H211" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Health", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$18:$B$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$18:$B$25)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$18:$C$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$18:$C$25)),1),IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$18:$D$25,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$18:$D$25)),1),Null))))</f>
-        <v>MoneyWasted</v>
+        <v>CrapStaff</v>
       </c>
       <c r="I211">
         <v>250</v>
@@ -11758,15 +11758,15 @@
       </c>
       <c r="F212" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F212" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>OurWayOrHiWay</v>
       </c>
       <c r="G212" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G212" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WEStrong</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="H212" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H212" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>JoinTheCAUSE</v>
+        <v>CommunityBuild</v>
       </c>
       <c r="I212">
         <v>75</v>
@@ -11802,7 +11802,7 @@
       </c>
       <c r="F213" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F213" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>ALWAYSSupport</v>
+        <v>JoinTheCAUSE</v>
       </c>
       <c r="G213" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G213" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -11810,7 +11810,7 @@
       </c>
       <c r="H213" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H213" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>OurWayOrHiWay</v>
+        <v>RallyTogether!</v>
       </c>
       <c r="I213">
         <v>50</v>
@@ -11846,7 +11846,7 @@
       </c>
       <c r="F214" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F214" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Desperate</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="G214" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G214" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -11854,7 +11854,7 @@
       </c>
       <c r="H214" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H214" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>WeNeedChange</v>
+        <v>Desperate</v>
       </c>
       <c r="I214">
         <v>150</v>
@@ -11890,15 +11890,15 @@
       </c>
       <c r="F215" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F215" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>TimeToFixIt</v>
+        <v>Desperate</v>
       </c>
       <c r="G215" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G215" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>AlwaysThem</v>
       </c>
       <c r="H215" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H215" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Outcast</v>
+        <v>TimeToFixIt</v>
       </c>
       <c r="I215">
         <v>200</v>
@@ -11938,11 +11938,11 @@
       </c>
       <c r="G216" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G216" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>NecessaryEvil</v>
       </c>
       <c r="H216" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H216" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>OurLastHope</v>
       </c>
       <c r="I216">
         <v>400</v>
@@ -11978,7 +11978,7 @@
       </c>
       <c r="F217" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="F217" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>Messiah</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="G217" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="G217" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
@@ -11986,7 +11986,7 @@
       </c>
       <c r="H217" s="7" t="str" cm="1">
         <f t="array" aca="1" ref="H217" ca="1">IF(Table1[[#This Row],[Subject (Government, Violence, Health, Radicalism)]] ="Radicalism", IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Happy", INDEX('Hashtag Source'!$B$26:$B$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$B$26:$B$32)),1), IF(Table1[[#This Row],[Reaction (Happy, Sad, Angry)]] = "Sad", INDEX('Hashtag Source'!$C$26:$C$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$C$26:$C$32)),1),IF( Table1[[#This Row],[Reaction (Happy, Sad, Angry)]]= "Angry", INDEX('Hashtag Source'!$D$26:$D$32,RANDBETWEEN(1,ROWS('Hashtag Source'!$D$26:$D$32)),1),Null))))</f>
-        <v>AgainstUS!!</v>
+        <v>MartyrUS!!</v>
       </c>
       <c r="I217">
         <v>150</v>
@@ -12499,7 +12499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C29F16F-EAFE-4B18-A8CA-D239C88544B3}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -14113,8 +14113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD59F98-9E92-490C-932F-B482BEFC87E4}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14225,7 +14225,7 @@
         <v>470</v>
       </c>
       <c r="E6" t="s">
-        <v>427</v>
+        <v>472</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -14767,7 +14767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53B4979-BA2F-42C6-BF9E-77AF10AFAE50}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>

</xml_diff>